<commit_message>
Quests Definitions Tabel Added
Former-commit-id: 37933866552c63aaa31cebb2f85940080fed7cd1
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tournaments" sheetId="2" r:id="rId1"/>
+    <sheet name="quests" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="247">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -584,6 +585,189 @@
   </si>
   <si>
     <t>icon_golden</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_PUMPKINS</t>
+  </si>
+  <si>
+    <t>season_halloween_0;season_halloween_1;season_halloween_2;</t>
+  </si>
+  <si>
+    <t>Pumpkins</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_HEARTS</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_COLLECT_EGG</t>
+  </si>
+  <si>
+    <t>egg_standard</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_SHAMROCK</t>
+  </si>
+  <si>
+    <t>st_patrick_balloon</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_FIRST_DAY_SUMMER_WATERMELONS</t>
+  </si>
+  <si>
+    <t>PreSummer_02_watermelon</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_EAT_FLYINGBUNNIES</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_GIFT</t>
+  </si>
+  <si>
+    <t>XmasPresent</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_DESTROY_HOUSES</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_DIVE</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_RED_ENVELOPE</t>
+  </si>
+  <si>
+    <t>red_envelop</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_SURVIVE_TIME</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_COLLECT_COINS</t>
+  </si>
+  <si>
+    <t>valentines_heart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TID_GLOBAL_EVENT_HUNGRY_BIRTHDAY </t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_EAT_BIRDS</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_SCORE</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_DISTANCE</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_EASTER_BUNNIES</t>
+  </si>
+  <si>
+    <t>easter_bunny</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_BIRTHDAY_CANDLES</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_FIRERUSH</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_BIRTHDAY_HATS</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_EAT_PEPPER</t>
+  </si>
+  <si>
+    <t>MexicanPepper</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_FIRST_DAY_SUMMER</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_BIRTHDAY_CAKES</t>
+  </si>
+  <si>
+    <t>Anniversary1_Cake_Piece</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_EAT_FLYING_PIGS</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_EAT_ARCHER</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_FOOTBALL</t>
+  </si>
+  <si>
+    <t>football_ball</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_EAT_GOBLINS</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_EAT_DRAGONS</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_EAT_FISH</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_EAT_GHOSTS</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_EAT_SPIDERS</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_EAT_TROLLS</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_EAT_FAIRIES</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_EAT_HUMANS</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_EAT_GOLDEN</t>
+  </si>
+  <si>
+    <t>icon_pumpkin</t>
+  </si>
+  <si>
+    <t>icon_heart</t>
+  </si>
+  <si>
+    <t>icon_egg</t>
+  </si>
+  <si>
+    <t>icon_stpatrick_balloon</t>
+  </si>
+  <si>
+    <t>icon_watermelon</t>
+  </si>
+  <si>
+    <t>icon_mission_destroy_gift</t>
+  </si>
+  <si>
+    <t>icon_red_envelope</t>
+  </si>
+  <si>
+    <t>icon_easter_bunny</t>
+  </si>
+  <si>
+    <t>icon_mexican_pepper</t>
+  </si>
+  <si>
+    <t>icon_football</t>
+  </si>
+  <si>
+    <t>icon_spiders</t>
+  </si>
+  <si>
+    <t>icon_eat_gold</t>
+  </si>
+  <si>
+    <t>{questsDefinitions}</t>
+  </si>
+  <si>
+    <t>QUESTS DEFINITIONS</t>
   </si>
 </sst>
 </file>
@@ -1028,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3104,4 +3288,701 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="73.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="4" max="4" width="128.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="8"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="12" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="12" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="12" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="E30" s="9"/>
+      <c r="F30" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="9"/>
+      <c r="F36" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="10"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="12" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Tournament Excel Content
Former-commit-id: 5864a32aa547054cca82b4968f213a07d57f5640
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="265">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -768,13 +768,67 @@
   </si>
   <si>
     <t>QUESTS DEFINITIONS</t>
+  </si>
+  <si>
+    <t>Villager01;boatrider;Bakerwoman;Villager04;Villager03;Villager02;Troll;Miner</t>
+  </si>
+  <si>
+    <t>icon_humans_halloween</t>
+  </si>
+  <si>
+    <t>Ground_Zombie</t>
+  </si>
+  <si>
+    <t>icon_grave_zombie</t>
+  </si>
+  <si>
+    <t>*TID_HALLOWEEN_SCISSORS_HAT;*TID_HALLOWEEN__FRANK_MASK;*TID_HALLOWEEN_VAMPIRE_MASK;*TID_HALLOWEEN__AXE_HAT;*TID_HALLOWEEN__SAW_HAT;*TID_HALLOWEEN__WEREWOLF_MASK;*TID_HALLOWEEN__WITCH_HAT;*TID_HALLOWEEN__SKULL_MASK;*TID_HALLOWEEN__PITCHFORK_HAT;</t>
+  </si>
+  <si>
+    <t>Halloween</t>
+  </si>
+  <si>
+    <t>icon_masks_halloween</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_ZOMBIES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_ZOMBIES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_ZOMBIES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_GRAVES_ZOMBIES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_GRAVES_ZOMBIES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_GRAVES_ZOMBIES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_WEARING_NORMAL_HALLOWEEN</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_WEARING_TIME_LIMIT_HALLOWEEN</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_WEARING_TIME_ATTACK_HALLOWEEN</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_ZOMBIES</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_GRAVES_ZOMBIES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -813,6 +867,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF172B4D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -840,7 +907,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -896,11 +963,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -929,6 +1009,22 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1210,10 +1306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3284,6 +3380,201 @@
         <v>185</v>
       </c>
     </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B100" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" s="9">
+        <v>0</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="F100" s="9"/>
+      <c r="G100" s="12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" s="9">
+        <v>2</v>
+      </c>
+      <c r="E101" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="F101" s="9"/>
+      <c r="G101" s="12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B102" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102" s="9">
+        <v>1</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="F102" s="9"/>
+      <c r="G102" s="12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B103" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D103" s="9">
+        <v>0</v>
+      </c>
+      <c r="E103" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F103" s="9"/>
+      <c r="G103" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B104" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C104" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D104" s="9">
+        <v>2</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F104" s="9"/>
+      <c r="G104" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B105" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105" s="9">
+        <v>1</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F105" s="9"/>
+      <c r="G105" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B106" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="C106" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D106" s="9">
+        <v>0</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="F106" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="G106" s="12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B107" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D107" s="9">
+        <v>2</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="F107" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="G107" s="12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B108" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D108" s="9">
+        <v>1</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="F108" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="G108" s="12" t="s">
+        <v>253</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3292,10 +3583,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3966,19 +4257,55 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="7" t="s">
+      <c r="A39" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="12" t="s">
+      <c r="C39" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="16"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="17" t="s">
         <v>244</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="E40" s="20"/>
+      <c r="F40" s="12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="E41" s="9"/>
+      <c r="F41" s="12" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tournament Excel Content Updated
Former-commit-id: 84e472b0bfa02f05dd856e4b9c2f7a9dd9067671
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -770,9 +770,6 @@
     <t>QUESTS DEFINITIONS</t>
   </si>
   <si>
-    <t>Villager01;boatrider;Bakerwoman;Villager04;Villager03;Villager02;Troll;Miner</t>
-  </si>
-  <si>
     <t>icon_humans_halloween</t>
   </si>
   <si>
@@ -822,6 +819,9 @@
   </si>
   <si>
     <t>TID_GLOBAL_EVENT_GRAVES_ZOMBIES</t>
+  </si>
+  <si>
+    <t>Villager01;boatrider;Bakerwoman</t>
   </si>
 </sst>
 </file>
@@ -980,7 +980,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1019,12 +1019,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1309,7 +1308,7 @@
   <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3385,7 +3384,7 @@
         <v>0</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C100" s="9" t="s">
         <v>7</v>
@@ -3394,11 +3393,11 @@
         <v>0</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="F100" s="9"/>
       <c r="G100" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3406,7 +3405,7 @@
         <v>0</v>
       </c>
       <c r="B101" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C101" s="9" t="s">
         <v>7</v>
@@ -3415,11 +3414,11 @@
         <v>2</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="F101" s="9"/>
       <c r="G101" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3427,7 +3426,7 @@
         <v>0</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C102" s="9" t="s">
         <v>7</v>
@@ -3436,11 +3435,11 @@
         <v>1</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="F102" s="9"/>
       <c r="G102" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3448,7 +3447,7 @@
         <v>0</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C103" s="9" t="s">
         <v>7</v>
@@ -3457,11 +3456,11 @@
         <v>0</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F103" s="9"/>
       <c r="G103" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3469,7 +3468,7 @@
         <v>0</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C104" s="9" t="s">
         <v>7</v>
@@ -3478,11 +3477,11 @@
         <v>2</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F104" s="9"/>
       <c r="G104" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3490,7 +3489,7 @@
         <v>0</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C105" s="9" t="s">
         <v>7</v>
@@ -3499,11 +3498,11 @@
         <v>1</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F105" s="9"/>
       <c r="G105" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3511,7 +3510,7 @@
         <v>0</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C106" s="9" t="s">
         <v>33</v>
@@ -3520,13 +3519,13 @@
         <v>0</v>
       </c>
       <c r="E106" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="F106" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="F106" s="9" t="s">
+      <c r="G106" s="12" t="s">
         <v>252</v>
-      </c>
-      <c r="G106" s="12" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3534,7 +3533,7 @@
         <v>0</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C107" s="9" t="s">
         <v>33</v>
@@ -3543,13 +3542,13 @@
         <v>2</v>
       </c>
       <c r="E107" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="F107" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="F107" s="9" t="s">
+      <c r="G107" s="12" t="s">
         <v>252</v>
-      </c>
-      <c r="G107" s="12" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3557,7 +3556,7 @@
         <v>0</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C108" s="9" t="s">
         <v>33</v>
@@ -3566,13 +3565,13 @@
         <v>1</v>
       </c>
       <c r="E108" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="F108" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="F108" s="9" t="s">
+      <c r="G108" s="12" t="s">
         <v>252</v>
-      </c>
-      <c r="G108" s="12" t="s">
-        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -3586,7 +3585,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4272,40 +4271,40 @@
         <v>244</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="E40" s="18"/>
+      <c r="F40" s="12" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="E40" s="20"/>
-      <c r="F40" s="12" t="s">
+      <c r="C41" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="19" t="s">
-        <v>264</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>249</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the tournaments table in content
Former-commit-id: 5ec48c7b0160cd97c75cdd41d2ebc79ab8bb85fb
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860"/>
   </bookViews>
   <sheets>
     <sheet name="tournaments" sheetId="2" r:id="rId1"/>
     <sheet name="quests" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="266">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -822,6 +822,9 @@
   </si>
   <si>
     <t>Villager01;boatrider;Bakerwoman</t>
+  </si>
+  <si>
+    <t>%all%</t>
   </si>
 </sst>
 </file>
@@ -980,7 +983,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1024,6 +1027,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1307,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,7 +2181,9 @@
       <c r="D41" s="9">
         <v>0</v>
       </c>
-      <c r="E41" s="9"/>
+      <c r="E41" s="20" t="s">
+        <v>265</v>
+      </c>
       <c r="F41" s="9"/>
       <c r="G41" s="11" t="s">
         <v>36</v>
@@ -2194,7 +2202,9 @@
       <c r="D42" s="9">
         <v>2</v>
       </c>
-      <c r="E42" s="9"/>
+      <c r="E42" s="20" t="s">
+        <v>265</v>
+      </c>
       <c r="F42" s="9"/>
       <c r="G42" s="11" t="s">
         <v>36</v>
@@ -2213,7 +2223,9 @@
       <c r="D43" s="9">
         <v>1</v>
       </c>
-      <c r="E43" s="9"/>
+      <c r="E43" s="20" t="s">
+        <v>265</v>
+      </c>
       <c r="F43" s="9"/>
       <c r="G43" s="11" t="s">
         <v>36</v>
@@ -2799,7 +2811,9 @@
       <c r="D71" s="9">
         <v>0</v>
       </c>
-      <c r="E71" s="9"/>
+      <c r="E71" s="20" t="s">
+        <v>265</v>
+      </c>
       <c r="F71" s="9"/>
       <c r="G71" s="9" t="s">
         <v>150</v>
@@ -2818,7 +2832,9 @@
       <c r="D72" s="9">
         <v>2</v>
       </c>
-      <c r="E72" s="9"/>
+      <c r="E72" s="20" t="s">
+        <v>265</v>
+      </c>
       <c r="F72" s="9"/>
       <c r="G72" s="9" t="s">
         <v>150</v>
@@ -2837,7 +2853,9 @@
       <c r="D73" s="9">
         <v>1</v>
       </c>
-      <c r="E73" s="9"/>
+      <c r="E73" s="20" t="s">
+        <v>265</v>
+      </c>
       <c r="F73" s="9"/>
       <c r="G73" s="9" t="s">
         <v>150</v>
@@ -2856,7 +2874,9 @@
       <c r="D74" s="9">
         <v>0</v>
       </c>
-      <c r="E74" s="9"/>
+      <c r="E74" s="20" t="s">
+        <v>265</v>
+      </c>
       <c r="F74" s="9"/>
       <c r="G74" s="9" t="s">
         <v>154</v>
@@ -2875,7 +2895,9 @@
       <c r="D75" s="9">
         <v>2</v>
       </c>
-      <c r="E75" s="9"/>
+      <c r="E75" s="20" t="s">
+        <v>265</v>
+      </c>
       <c r="F75" s="9"/>
       <c r="G75" s="9" t="s">
         <v>154</v>
@@ -2894,7 +2916,9 @@
       <c r="D76" s="9">
         <v>1</v>
       </c>
-      <c r="E76" s="9"/>
+      <c r="E76" s="20" t="s">
+        <v>265</v>
+      </c>
       <c r="F76" s="9"/>
       <c r="G76" s="9" t="s">
         <v>154</v>
@@ -3335,7 +3359,9 @@
       <c r="D97" s="9">
         <v>0</v>
       </c>
-      <c r="E97" s="9"/>
+      <c r="E97" s="20" t="s">
+        <v>265</v>
+      </c>
       <c r="F97" s="9"/>
       <c r="G97" s="9" t="s">
         <v>185</v>
@@ -3354,7 +3380,9 @@
       <c r="D98" s="9">
         <v>2</v>
       </c>
-      <c r="E98" s="9"/>
+      <c r="E98" s="20" t="s">
+        <v>265</v>
+      </c>
       <c r="F98" s="9"/>
       <c r="G98" s="9" t="s">
         <v>185</v>
@@ -3373,7 +3401,9 @@
       <c r="D99" s="9">
         <v>1</v>
       </c>
-      <c r="E99" s="9"/>
+      <c r="E99" s="20" t="s">
+        <v>265</v>
+      </c>
       <c r="F99" s="9"/>
       <c r="G99" s="9" t="s">
         <v>185</v>
@@ -3584,7 +3614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated the tournament content
Former-commit-id: b308a6207143bf2a90e80ba8adbc86bc6b820fbf
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="271">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -431,9 +431,6 @@
     <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_STPATRICK</t>
   </si>
   <si>
-    <t>*TID_LEPRECHAUN_HAT</t>
-  </si>
-  <si>
     <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_TROLLS</t>
   </si>
   <si>
@@ -452,9 +449,6 @@
     <t>TID_EVENT_TOURNAMENT_WEARING_KILL_TIME_ATTACK_UFO_DAY_DISGUISE</t>
   </si>
   <si>
-    <t>*TID_ALIEN_MASK ; TID_FOIL_PAPER_HAT</t>
-  </si>
-  <si>
     <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_WITCHES</t>
   </si>
   <si>
@@ -779,9 +773,6 @@
     <t>icon_grave_zombie</t>
   </si>
   <si>
-    <t>*TID_HALLOWEEN_SCISSORS_HAT;*TID_HALLOWEEN__FRANK_MASK;*TID_HALLOWEEN_VAMPIRE_MASK;*TID_HALLOWEEN__AXE_HAT;*TID_HALLOWEEN__SAW_HAT;*TID_HALLOWEEN__WEREWOLF_MASK;*TID_HALLOWEEN__WITCH_HAT;*TID_HALLOWEEN__SKULL_MASK;*TID_HALLOWEEN__PITCHFORK_HAT;</t>
-  </si>
-  <si>
     <t>Halloween</t>
   </si>
   <si>
@@ -825,6 +816,30 @@
   </si>
   <si>
     <t>%all%</t>
+  </si>
+  <si>
+    <t>leprechaun_hat</t>
+  </si>
+  <si>
+    <t>anniversary_hat</t>
+  </si>
+  <si>
+    <t>halloween_scissors_hat;halloween_frank_mask;halloween_vampire_mask;halloween_axe_hat;halloween_saw_hat;halloween_werewolf_mask;halloween_witch_hat;halloween_skull_mask;halloween_pitchfork_hat</t>
+  </si>
+  <si>
+    <t>alien_mask;Foil_Paper_hat</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_WEARING_NORMAL_CHRISTMAS_HAT</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_WEARING_TIME_LIMIT_CHRISTMAS_HAT</t>
+  </si>
+  <si>
+    <t>christmas_santa_hat</t>
+  </si>
+  <si>
+    <t>icon_XmasHat</t>
   </si>
 </sst>
 </file>
@@ -983,7 +998,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1030,6 +1045,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1311,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E118" sqref="E118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,7 +1341,7 @@
     <col min="2" max="2" width="73.85546875" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="5" max="5" width="128.85546875" customWidth="1"/>
+    <col min="5" max="5" width="198.5703125" customWidth="1"/>
     <col min="6" max="6" width="27.140625" customWidth="1"/>
     <col min="7" max="7" width="32.7109375" customWidth="1"/>
   </cols>
@@ -1750,7 +1768,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="11" t="s">
@@ -1771,7 +1789,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="11" t="s">
@@ -1792,7 +1810,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="11" t="s">
@@ -1807,7 +1825,7 @@
         <v>83</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D24" s="9">
         <v>0</v>
@@ -1828,7 +1846,7 @@
         <v>84</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D25" s="9">
         <v>2</v>
@@ -2182,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="11" t="s">
@@ -2203,7 +2221,7 @@
         <v>2</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="11" t="s">
@@ -2224,7 +2242,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="11" t="s">
@@ -2371,7 +2389,7 @@
         <v>121</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D50" s="9">
         <v>0</v>
@@ -2392,7 +2410,7 @@
         <v>122</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D51" s="9">
         <v>2</v>
@@ -2413,7 +2431,7 @@
         <v>123</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D52" s="9">
         <v>1</v>
@@ -2554,7 +2572,7 @@
         <v>0</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>134</v>
+        <v>263</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="11" t="s">
@@ -2575,7 +2593,7 @@
         <v>2</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>134</v>
+        <v>263</v>
       </c>
       <c r="F60" s="9"/>
       <c r="G60" s="11" t="s">
@@ -2596,7 +2614,7 @@
         <v>1</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>134</v>
+        <v>263</v>
       </c>
       <c r="F61" s="9"/>
       <c r="G61" s="11" t="s">
@@ -2608,7 +2626,7 @@
         <v>0</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>7</v>
@@ -2629,7 +2647,7 @@
         <v>0</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C63" s="9" t="s">
         <v>7</v>
@@ -2650,7 +2668,7 @@
         <v>0</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>7</v>
@@ -2671,7 +2689,7 @@
         <v>0</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C65" s="9" t="s">
         <v>33</v>
@@ -2680,7 +2698,7 @@
         <v>0</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>141</v>
+        <v>266</v>
       </c>
       <c r="F65" s="9"/>
       <c r="G65" s="11" t="s">
@@ -2692,7 +2710,7 @@
         <v>0</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>33</v>
@@ -2701,7 +2719,7 @@
         <v>2</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>141</v>
+        <v>266</v>
       </c>
       <c r="F66" s="9"/>
       <c r="G66" s="11" t="s">
@@ -2713,7 +2731,7 @@
         <v>0</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C67" s="9" t="s">
         <v>33</v>
@@ -2722,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>141</v>
+        <v>266</v>
       </c>
       <c r="F67" s="9"/>
       <c r="G67" s="11" t="s">
@@ -2734,7 +2752,7 @@
         <v>0</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C68" s="9" t="s">
         <v>7</v>
@@ -2743,10 +2761,10 @@
         <v>0</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G68" s="11" t="s">
         <v>42</v>
@@ -2757,7 +2775,7 @@
         <v>0</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C69" s="9" t="s">
         <v>7</v>
@@ -2766,10 +2784,10 @@
         <v>2</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G69" s="11" t="s">
         <v>42</v>
@@ -2780,7 +2798,7 @@
         <v>0</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>7</v>
@@ -2789,10 +2807,10 @@
         <v>1</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G70" s="11" t="s">
         <v>42</v>
@@ -2803,7 +2821,7 @@
         <v>0</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C71" s="9" t="s">
         <v>30</v>
@@ -2812,11 +2830,11 @@
         <v>0</v>
       </c>
       <c r="E71" s="20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F71" s="9"/>
       <c r="G71" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2824,7 +2842,7 @@
         <v>0</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C72" s="9" t="s">
         <v>30</v>
@@ -2833,11 +2851,11 @@
         <v>2</v>
       </c>
       <c r="E72" s="20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F72" s="9"/>
       <c r="G72" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2845,7 +2863,7 @@
         <v>0</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>30</v>
@@ -2854,11 +2872,11 @@
         <v>1</v>
       </c>
       <c r="E73" s="20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F73" s="9"/>
       <c r="G73" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2866,7 +2884,7 @@
         <v>0</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>32</v>
@@ -2875,11 +2893,11 @@
         <v>0</v>
       </c>
       <c r="E74" s="20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F74" s="9"/>
       <c r="G74" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2887,7 +2905,7 @@
         <v>0</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C75" s="9" t="s">
         <v>32</v>
@@ -2896,11 +2914,11 @@
         <v>2</v>
       </c>
       <c r="E75" s="20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F75" s="9"/>
       <c r="G75" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2908,7 +2926,7 @@
         <v>0</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>32</v>
@@ -2917,11 +2935,11 @@
         <v>1</v>
       </c>
       <c r="E76" s="20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F76" s="9"/>
       <c r="G76" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2929,7 +2947,7 @@
         <v>0</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C77" s="12" t="s">
         <v>46</v>
@@ -2967,7 +2985,7 @@
         <v>0</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>46</v>
@@ -2986,7 +3004,7 @@
         <v>0</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C80" s="12" t="s">
         <v>48</v>
@@ -3024,7 +3042,7 @@
         <v>0</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C82" s="9" t="s">
         <v>7</v>
@@ -3033,13 +3051,13 @@
         <v>0</v>
       </c>
       <c r="E82" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F82" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="F82" s="9" t="s">
-        <v>164</v>
-      </c>
       <c r="G82" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3047,7 +3065,7 @@
         <v>0</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>7</v>
@@ -3056,13 +3074,13 @@
         <v>2</v>
       </c>
       <c r="E83" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F83" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="F83" s="9" t="s">
-        <v>164</v>
-      </c>
       <c r="G83" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3070,7 +3088,7 @@
         <v>0</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C84" s="9" t="s">
         <v>7</v>
@@ -3079,13 +3097,13 @@
         <v>1</v>
       </c>
       <c r="E84" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F84" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="F84" s="9" t="s">
-        <v>164</v>
-      </c>
       <c r="G84" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3093,7 +3111,7 @@
         <v>0</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C85" s="9" t="s">
         <v>7</v>
@@ -3114,7 +3132,7 @@
         <v>0</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C86" s="9" t="s">
         <v>7</v>
@@ -3135,7 +3153,7 @@
         <v>0</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C87" s="9" t="s">
         <v>7</v>
@@ -3156,19 +3174,19 @@
         <v>0</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D88" s="9">
         <v>0</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G88" s="11" t="s">
         <v>39</v>
@@ -3179,19 +3197,19 @@
         <v>0</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D89" s="9">
         <v>2</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F89" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G89" s="11" t="s">
         <v>39</v>
@@ -3202,19 +3220,19 @@
         <v>0</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D90" s="9">
         <v>1</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G90" s="11" t="s">
         <v>39</v>
@@ -3225,16 +3243,16 @@
         <v>0</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D91" s="9">
         <v>0</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F91" s="9"/>
       <c r="G91" s="11" t="s">
@@ -3246,16 +3264,16 @@
         <v>0</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D92" s="9">
         <v>2</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F92" s="9"/>
       <c r="G92" s="11" t="s">
@@ -3267,16 +3285,16 @@
         <v>0</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D93" s="9">
         <v>1</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F93" s="9"/>
       <c r="G93" s="11" t="s">
@@ -3288,7 +3306,7 @@
         <v>0</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C94" s="9" t="s">
         <v>33</v>
@@ -3297,7 +3315,7 @@
         <v>0</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>180</v>
+        <v>264</v>
       </c>
       <c r="F94" s="9"/>
       <c r="G94" s="11" t="s">
@@ -3309,7 +3327,7 @@
         <v>0</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C95" s="9" t="s">
         <v>33</v>
@@ -3318,7 +3336,7 @@
         <v>2</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>180</v>
+        <v>264</v>
       </c>
       <c r="F95" s="9"/>
       <c r="G95" s="11" t="s">
@@ -3330,7 +3348,7 @@
         <v>0</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C96" s="9" t="s">
         <v>33</v>
@@ -3339,7 +3357,7 @@
         <v>1</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>180</v>
+        <v>264</v>
       </c>
       <c r="F96" s="9"/>
       <c r="G96" s="11" t="s">
@@ -3351,20 +3369,20 @@
         <v>0</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D97" s="9">
         <v>0</v>
       </c>
       <c r="E97" s="20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F97" s="9"/>
       <c r="G97" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3372,20 +3390,20 @@
         <v>0</v>
       </c>
       <c r="B98" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C98" s="9" t="s">
         <v>182</v>
-      </c>
-      <c r="C98" s="9" t="s">
-        <v>184</v>
       </c>
       <c r="D98" s="9">
         <v>2</v>
       </c>
       <c r="E98" s="20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F98" s="9"/>
       <c r="G98" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3393,20 +3411,20 @@
         <v>0</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D99" s="9">
         <v>1</v>
       </c>
       <c r="E99" s="20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F99" s="9"/>
       <c r="G99" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3414,7 +3432,7 @@
         <v>0</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C100" s="9" t="s">
         <v>7</v>
@@ -3423,11 +3441,11 @@
         <v>0</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F100" s="9"/>
       <c r="G100" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3435,7 +3453,7 @@
         <v>0</v>
       </c>
       <c r="B101" s="13" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C101" s="9" t="s">
         <v>7</v>
@@ -3444,11 +3462,11 @@
         <v>2</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F101" s="9"/>
       <c r="G101" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3456,7 +3474,7 @@
         <v>0</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C102" s="9" t="s">
         <v>7</v>
@@ -3465,11 +3483,11 @@
         <v>1</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F102" s="9"/>
       <c r="G102" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3477,7 +3495,7 @@
         <v>0</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C103" s="9" t="s">
         <v>7</v>
@@ -3486,11 +3504,11 @@
         <v>0</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F103" s="9"/>
       <c r="G103" s="12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3498,7 +3516,7 @@
         <v>0</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C104" s="9" t="s">
         <v>7</v>
@@ -3507,11 +3525,11 @@
         <v>2</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F104" s="9"/>
       <c r="G104" s="12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3519,7 +3537,7 @@
         <v>0</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C105" s="9" t="s">
         <v>7</v>
@@ -3528,11 +3546,11 @@
         <v>1</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F105" s="9"/>
       <c r="G105" s="12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3540,7 +3558,7 @@
         <v>0</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C106" s="9" t="s">
         <v>33</v>
@@ -3549,13 +3567,13 @@
         <v>0</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="F106" s="9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G106" s="12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3563,7 +3581,7 @@
         <v>0</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C107" s="9" t="s">
         <v>33</v>
@@ -3572,13 +3590,13 @@
         <v>2</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G107" s="12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3586,7 +3604,7 @@
         <v>0</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C108" s="9" t="s">
         <v>33</v>
@@ -3595,13 +3613,55 @@
         <v>1</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G108" s="12" t="s">
-        <v>252</v>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D109" s="9">
+        <v>0</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="F109" s="9"/>
+      <c r="G109" s="21" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B110" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D110" s="9">
+        <v>2</v>
+      </c>
+      <c r="E110" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="F110" s="9"/>
+      <c r="G110" s="21" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -3631,7 +3691,7 @@
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3647,7 +3707,7 @@
     </row>
     <row r="4" spans="1:6" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -3670,19 +3730,19 @@
         <v>0</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3690,17 +3750,17 @@
         <v>0</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3708,17 +3768,17 @@
         <v>0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3726,17 +3786,17 @@
         <v>0</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3744,17 +3804,17 @@
         <v>0</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3762,13 +3822,13 @@
         <v>0</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="12" t="s">
@@ -3780,17 +3840,17 @@
         <v>0</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="12" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3798,7 +3858,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>29</v>
@@ -3818,7 +3878,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>2</v>
@@ -3834,17 +3894,17 @@
         <v>0</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3852,7 +3912,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>4</v>
@@ -3868,7 +3928,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>3</v>
@@ -3886,7 +3946,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>46</v>
@@ -3902,7 +3962,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>7</v>
@@ -3922,7 +3982,7 @@
         <v>0</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>5</v>
@@ -3938,7 +3998,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>2</v>
@@ -3954,17 +4014,17 @@
         <v>0</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -3972,13 +4032,13 @@
         <v>0</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="12" t="s">
@@ -3990,7 +4050,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>6</v>
@@ -4006,13 +4066,13 @@
         <v>0</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="12" t="s">
@@ -4024,17 +4084,17 @@
         <v>0</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="12" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4042,13 +4102,13 @@
         <v>0</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="12" t="s">
@@ -4060,13 +4120,13 @@
         <v>0</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="12" t="s">
@@ -4078,7 +4138,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>7</v>
@@ -4096,7 +4156,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>7</v>
@@ -4114,17 +4174,17 @@
         <v>0</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4132,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>7</v>
@@ -4152,7 +4212,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>7</v>
@@ -4172,7 +4232,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>7</v>
@@ -4192,7 +4252,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>7</v>
@@ -4212,7 +4272,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>7</v>
@@ -4224,7 +4284,7 @@
         <v>108</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -4232,7 +4292,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>7</v>
@@ -4250,19 +4310,19 @@
         <v>0</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D37" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E37" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="E37" s="9" t="s">
-        <v>164</v>
-      </c>
       <c r="F37" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -4270,7 +4330,7 @@
         <v>0</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>7</v>
@@ -4290,7 +4350,7 @@
         <v>0</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>7</v>
@@ -4298,7 +4358,7 @@
       <c r="D39" s="16"/>
       <c r="E39" s="14"/>
       <c r="F39" s="17" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -4306,17 +4366,17 @@
         <v>0</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E40" s="18"/>
       <c r="F40" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -4324,17 +4384,17 @@
         <v>0</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small fix on the tournaments content.
Former-commit-id: 6eb4d89801e5c674bf8eceb6a5837dc245fd6c01
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -15,7 +15,7 @@
     <sheet name="tournaments" sheetId="2" r:id="rId1"/>
     <sheet name="quests" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="288">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -840,13 +840,64 @@
   </si>
   <si>
     <t>icon_XmasHat</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NIAN_TIME_LIMIT</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NIAN_NORMAL</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NIAN_TIME_ATTACK</t>
+  </si>
+  <si>
+    <t>Nian</t>
+  </si>
+  <si>
+    <t>icon_nian</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_CATTLE_NORMAL</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_CATTLE_TIME_ATTACK</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_CATTLE_TIME_LIMIT</t>
+  </si>
+  <si>
+    <t>Cow;Horse;Sheep;</t>
+  </si>
+  <si>
+    <t>icon_sheep</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_EAT_TIME_LIMIT_GINGERBREAD_MAN_COOKIE</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_EAT_NORMAL_GINGERBREAD_MAN_COOKIE</t>
+  </si>
+  <si>
+    <t>GingerbreadManCookie</t>
+  </si>
+  <si>
+    <t>icon_GingerbreadManCookie</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_NIAN</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_CHRISTMAS_HAT</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_GINGERBREAD_MAN_COOKIE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -898,6 +949,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -925,7 +982,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -994,11 +1051,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1049,6 +1119,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1329,10 +1417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G110"/>
+  <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E118" sqref="E118"/>
+    <sheetView tabSelected="1" topLeftCell="E85" workbookViewId="0">
+      <selection activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3647,7 +3735,7 @@
       <c r="A110" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B110" s="13" t="s">
+      <c r="B110" s="23" t="s">
         <v>268</v>
       </c>
       <c r="C110" s="9" t="s">
@@ -3663,6 +3751,251 @@
       <c r="G110" s="21" t="s">
         <v>270</v>
       </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B111" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D111" s="9">
+        <v>2</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="F111" s="9"/>
+      <c r="G111" s="9" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B112" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="C112" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112" s="9">
+        <v>0</v>
+      </c>
+      <c r="E112" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="F112" s="9"/>
+      <c r="G112" s="9" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B113" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="C113" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D113" s="9">
+        <v>1</v>
+      </c>
+      <c r="E113" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="F113" s="9"/>
+      <c r="G113" s="9" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B114" s="25" t="s">
+        <v>278</v>
+      </c>
+      <c r="C114" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D114" s="9">
+        <v>2</v>
+      </c>
+      <c r="E114" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="F114" s="9"/>
+      <c r="G114" s="12" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B115" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="C115" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D115" s="9">
+        <v>0</v>
+      </c>
+      <c r="E115" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="F115" s="9"/>
+      <c r="G115" s="12" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B116" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="C116" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D116" s="9">
+        <v>1</v>
+      </c>
+      <c r="E116" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="F116" s="9"/>
+      <c r="G116" s="12" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="C117" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D117" s="22">
+        <v>2</v>
+      </c>
+      <c r="E117" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="F117" s="9"/>
+      <c r="G117" s="12" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B118" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="C118" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D118" s="22">
+        <v>0</v>
+      </c>
+      <c r="E118" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="F118" s="9"/>
+      <c r="G118" s="12" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B119" s="27"/>
+      <c r="C119" s="12"/>
+      <c r="D119" s="9"/>
+      <c r="E119" s="7"/>
+      <c r="F119" s="9"/>
+      <c r="G119" s="9"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B120" s="24"/>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="7"/>
+      <c r="F120" s="9"/>
+      <c r="G120" s="21"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B121" s="13"/>
+      <c r="C121" s="9"/>
+      <c r="D121" s="9"/>
+      <c r="E121" s="7"/>
+      <c r="F121" s="9"/>
+      <c r="G121" s="21"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B122" s="13"/>
+      <c r="C122" s="9"/>
+      <c r="D122" s="9"/>
+      <c r="E122" s="7"/>
+      <c r="F122" s="9"/>
+      <c r="G122" s="21"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B123" s="13"/>
+      <c r="C123" s="9"/>
+      <c r="D123" s="9"/>
+      <c r="E123" s="7"/>
+      <c r="F123" s="9"/>
+      <c r="G123" s="21"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B124" s="13"/>
+      <c r="C124" s="9"/>
+      <c r="D124" s="9"/>
+      <c r="E124" s="7"/>
+      <c r="F124" s="9"/>
+      <c r="G124" s="21"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B125" s="13"/>
+      <c r="C125" s="9"/>
+      <c r="D125" s="9"/>
+      <c r="E125" s="7"/>
+      <c r="F125" s="9"/>
+      <c r="G125" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3672,10 +4005,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4397,6 +4730,90 @@
         <v>247</v>
       </c>
     </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="E43" s="9"/>
+      <c r="F43" s="21" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="E44" s="9"/>
+      <c r="F44" s="12" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="19"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="12"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="19"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="12"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="19"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="12"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixing a row quest that had a last ";"
Former-commit-id: 30c61602f0367eed1add7c39a04df6dfce758ac6
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -584,9 +584,6 @@
     <t>TID_GLOBAL_EVENT_PUMPKINS</t>
   </si>
   <si>
-    <t>season_halloween_0;season_halloween_1;season_halloween_2;</t>
-  </si>
-  <si>
     <t>Pumpkins</t>
   </si>
   <si>
@@ -900,6 +897,9 @@
   </si>
   <si>
     <t>score_type</t>
+  </si>
+  <si>
+    <t>season_halloween_0;season_halloween_1;season_halloween_2</t>
   </si>
 </sst>
 </file>
@@ -1702,7 +1702,7 @@
         <v>70</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D14" s="9">
         <v>0</v>
@@ -2297,7 +2297,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="11" t="s">
@@ -2318,7 +2318,7 @@
         <v>2</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="11" t="s">
@@ -2339,7 +2339,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="11" t="s">
@@ -2549,7 +2549,7 @@
         <v>125</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D53" s="9">
         <v>0</v>
@@ -2568,7 +2568,7 @@
         <v>126</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D54" s="9">
         <v>2</v>
@@ -2587,7 +2587,7 @@
         <v>127</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D55" s="9">
         <v>1</v>
@@ -2606,7 +2606,7 @@
         <v>128</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D56" s="9">
         <v>0</v>
@@ -2625,7 +2625,7 @@
         <v>129</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D57" s="9">
         <v>2</v>
@@ -2644,7 +2644,7 @@
         <v>130</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D58" s="9">
         <v>1</v>
@@ -2669,7 +2669,7 @@
         <v>0</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="11" t="s">
@@ -2690,7 +2690,7 @@
         <v>2</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F60" s="9"/>
       <c r="G60" s="11" t="s">
@@ -2711,7 +2711,7 @@
         <v>1</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F61" s="9"/>
       <c r="G61" s="11" t="s">
@@ -2795,7 +2795,7 @@
         <v>0</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F65" s="9"/>
       <c r="G65" s="11" t="s">
@@ -2816,7 +2816,7 @@
         <v>2</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F66" s="9"/>
       <c r="G66" s="11" t="s">
@@ -2837,7 +2837,7 @@
         <v>1</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F67" s="9"/>
       <c r="G67" s="11" t="s">
@@ -2927,7 +2927,7 @@
         <v>0</v>
       </c>
       <c r="E71" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F71" s="9"/>
       <c r="G71" s="9" t="s">
@@ -2948,7 +2948,7 @@
         <v>2</v>
       </c>
       <c r="E72" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F72" s="9"/>
       <c r="G72" s="9" t="s">
@@ -2969,7 +2969,7 @@
         <v>1</v>
       </c>
       <c r="E73" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F73" s="9"/>
       <c r="G73" s="9" t="s">
@@ -2990,7 +2990,7 @@
         <v>0</v>
       </c>
       <c r="E74" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F74" s="9"/>
       <c r="G74" s="9" t="s">
@@ -3011,7 +3011,7 @@
         <v>2</v>
       </c>
       <c r="E75" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F75" s="9"/>
       <c r="G75" s="9" t="s">
@@ -3032,7 +3032,7 @@
         <v>1</v>
       </c>
       <c r="E76" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F76" s="9"/>
       <c r="G76" s="9" t="s">
@@ -3412,7 +3412,7 @@
         <v>0</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F94" s="9"/>
       <c r="G94" s="11" t="s">
@@ -3433,7 +3433,7 @@
         <v>2</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F95" s="9"/>
       <c r="G95" s="11" t="s">
@@ -3454,7 +3454,7 @@
         <v>1</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F96" s="9"/>
       <c r="G96" s="11" t="s">
@@ -3475,7 +3475,7 @@
         <v>0</v>
       </c>
       <c r="E97" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F97" s="9"/>
       <c r="G97" s="9" t="s">
@@ -3496,7 +3496,7 @@
         <v>2</v>
       </c>
       <c r="E98" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F98" s="9"/>
       <c r="G98" s="9" t="s">
@@ -3517,7 +3517,7 @@
         <v>1</v>
       </c>
       <c r="E99" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F99" s="9"/>
       <c r="G99" s="9" t="s">
@@ -3529,7 +3529,7 @@
         <v>0</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C100" s="9" t="s">
         <v>7</v>
@@ -3538,11 +3538,11 @@
         <v>0</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F100" s="9"/>
       <c r="G100" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3550,7 +3550,7 @@
         <v>0</v>
       </c>
       <c r="B101" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C101" s="9" t="s">
         <v>7</v>
@@ -3559,11 +3559,11 @@
         <v>2</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F101" s="9"/>
       <c r="G101" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3571,7 +3571,7 @@
         <v>0</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C102" s="9" t="s">
         <v>7</v>
@@ -3580,11 +3580,11 @@
         <v>1</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F102" s="9"/>
       <c r="G102" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3592,7 +3592,7 @@
         <v>0</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C103" s="9" t="s">
         <v>7</v>
@@ -3601,11 +3601,11 @@
         <v>0</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F103" s="9"/>
       <c r="G103" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3613,7 +3613,7 @@
         <v>0</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C104" s="9" t="s">
         <v>7</v>
@@ -3622,11 +3622,11 @@
         <v>2</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F104" s="9"/>
       <c r="G104" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3634,7 +3634,7 @@
         <v>0</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C105" s="9" t="s">
         <v>7</v>
@@ -3643,11 +3643,11 @@
         <v>1</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F105" s="9"/>
       <c r="G105" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3655,7 +3655,7 @@
         <v>0</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C106" s="9" t="s">
         <v>33</v>
@@ -3664,13 +3664,13 @@
         <v>0</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F106" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="G106" s="12" t="s">
         <v>248</v>
-      </c>
-      <c r="G106" s="12" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3678,7 +3678,7 @@
         <v>0</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C107" s="9" t="s">
         <v>33</v>
@@ -3687,13 +3687,13 @@
         <v>2</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F107" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="G107" s="12" t="s">
         <v>248</v>
-      </c>
-      <c r="G107" s="12" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3701,7 +3701,7 @@
         <v>0</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C108" s="9" t="s">
         <v>33</v>
@@ -3710,13 +3710,13 @@
         <v>1</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F108" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="G108" s="12" t="s">
         <v>248</v>
-      </c>
-      <c r="G108" s="12" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -3724,7 +3724,7 @@
         <v>0</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C109" s="9" t="s">
         <v>33</v>
@@ -3733,11 +3733,11 @@
         <v>0</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F109" s="9"/>
       <c r="G109" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -3745,7 +3745,7 @@
         <v>0</v>
       </c>
       <c r="B110" s="23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C110" s="9" t="s">
         <v>33</v>
@@ -3754,11 +3754,11 @@
         <v>2</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F110" s="9"/>
       <c r="G110" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -3766,7 +3766,7 @@
         <v>0</v>
       </c>
       <c r="B111" s="25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C111" s="9" t="s">
         <v>7</v>
@@ -3775,11 +3775,11 @@
         <v>2</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F111" s="9"/>
       <c r="G111" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -3787,7 +3787,7 @@
         <v>0</v>
       </c>
       <c r="B112" s="25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C112" s="9" t="s">
         <v>7</v>
@@ -3796,11 +3796,11 @@
         <v>0</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F112" s="9"/>
       <c r="G112" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3808,7 +3808,7 @@
         <v>0</v>
       </c>
       <c r="B113" s="26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C113" s="9" t="s">
         <v>7</v>
@@ -3817,11 +3817,11 @@
         <v>1</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F113" s="9"/>
       <c r="G113" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -3829,7 +3829,7 @@
         <v>0</v>
       </c>
       <c r="B114" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C114" s="9" t="s">
         <v>7</v>
@@ -3838,11 +3838,11 @@
         <v>2</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F114" s="9"/>
       <c r="G114" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3850,7 +3850,7 @@
         <v>0</v>
       </c>
       <c r="B115" s="25" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C115" s="9" t="s">
         <v>7</v>
@@ -3859,11 +3859,11 @@
         <v>0</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F115" s="9"/>
       <c r="G115" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -3871,7 +3871,7 @@
         <v>0</v>
       </c>
       <c r="B116" s="26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C116" s="9" t="s">
         <v>7</v>
@@ -3880,11 +3880,11 @@
         <v>1</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F116" s="9"/>
       <c r="G116" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -3892,7 +3892,7 @@
         <v>0</v>
       </c>
       <c r="B117" s="27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C117" s="9" t="s">
         <v>7</v>
@@ -3901,11 +3901,11 @@
         <v>2</v>
       </c>
       <c r="E117" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F117" s="9"/>
       <c r="G117" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -3913,20 +3913,20 @@
         <v>0</v>
       </c>
       <c r="B118" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="C118" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D118" s="22">
+        <v>0</v>
+      </c>
+      <c r="E118" s="28" t="s">
         <v>282</v>
-      </c>
-      <c r="C118" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D118" s="22">
-        <v>0</v>
-      </c>
-      <c r="E118" s="28" t="s">
-        <v>283</v>
       </c>
       <c r="F118" s="9"/>
       <c r="G118" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -4016,8 +4016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4033,7 +4033,7 @@
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -4049,7 +4049,7 @@
     </row>
     <row r="4" spans="1:6" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -4078,13 +4078,13 @@
         <v>3</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>186</v>
-      </c>
       <c r="F5" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4092,17 +4092,17 @@
         <v>0</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4110,17 +4110,17 @@
         <v>0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4128,17 +4128,17 @@
         <v>0</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4146,17 +4146,17 @@
         <v>0</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -4164,7 +4164,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>7</v>
@@ -4182,17 +4182,17 @@
         <v>0</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -4200,7 +4200,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>29</v>
@@ -4220,7 +4220,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>2</v>
@@ -4236,17 +4236,17 @@
         <v>0</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -4254,7 +4254,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>4</v>
@@ -4270,7 +4270,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>3</v>
@@ -4288,7 +4288,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>46</v>
@@ -4304,7 +4304,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>7</v>
@@ -4324,7 +4324,7 @@
         <v>0</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>5</v>
@@ -4340,7 +4340,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>2</v>
@@ -4356,17 +4356,17 @@
         <v>0</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>208</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>209</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4374,7 +4374,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>7</v>
@@ -4392,7 +4392,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>6</v>
@@ -4408,7 +4408,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>33</v>
@@ -4426,17 +4426,17 @@
         <v>0</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4444,7 +4444,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>3</v>
@@ -4462,13 +4462,13 @@
         <v>0</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>216</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>217</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="12" t="s">
@@ -4480,7 +4480,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>7</v>
@@ -4498,7 +4498,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>7</v>
@@ -4516,17 +4516,17 @@
         <v>0</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4534,7 +4534,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>7</v>
@@ -4554,7 +4554,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>7</v>
@@ -4574,7 +4574,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>7</v>
@@ -4594,7 +4594,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>7</v>
@@ -4614,7 +4614,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>7</v>
@@ -4626,7 +4626,7 @@
         <v>108</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -4634,7 +4634,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>7</v>
@@ -4652,7 +4652,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>7</v>
@@ -4672,7 +4672,7 @@
         <v>0</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>7</v>
@@ -4692,7 +4692,7 @@
         <v>0</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>7</v>
@@ -4700,7 +4700,7 @@
       <c r="D39" s="16"/>
       <c r="E39" s="14"/>
       <c r="F39" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -4708,17 +4708,17 @@
         <v>0</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E40" s="18"/>
       <c r="F40" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -4726,17 +4726,17 @@
         <v>0</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -4744,17 +4744,17 @@
         <v>0</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -4762,17 +4762,17 @@
         <v>0</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -4780,17 +4780,17 @@
         <v>0</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixing in tournaments a row with extra ";"
Former-commit-id: bf2c1c89d282b0f4a4be983bd2e8db6ac64bc4ad
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860"/>
   </bookViews>
   <sheets>
     <sheet name="tournaments" sheetId="2" r:id="rId1"/>
@@ -863,9 +863,6 @@
     <t>TID_EVENT_TOURNAMENT_KILL_CATTLE_TIME_LIMIT</t>
   </si>
   <si>
-    <t>Cow;Horse;Sheep;</t>
-  </si>
-  <si>
     <t>icon_sheep</t>
   </si>
   <si>
@@ -900,6 +897,9 @@
   </si>
   <si>
     <t>season_halloween_0;season_halloween_1;season_halloween_2</t>
+  </si>
+  <si>
+    <t>Cow;Horse;Sheep</t>
   </si>
 </sst>
 </file>
@@ -1428,8 +1428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="C80" workbookViewId="0">
+      <selection activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1702,7 +1702,7 @@
         <v>70</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D14" s="9">
         <v>0</v>
@@ -2549,7 +2549,7 @@
         <v>125</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D53" s="9">
         <v>0</v>
@@ -2568,7 +2568,7 @@
         <v>126</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D54" s="9">
         <v>2</v>
@@ -2587,7 +2587,7 @@
         <v>127</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D55" s="9">
         <v>1</v>
@@ -2606,7 +2606,7 @@
         <v>128</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D56" s="9">
         <v>0</v>
@@ -2625,7 +2625,7 @@
         <v>129</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D57" s="9">
         <v>2</v>
@@ -2644,7 +2644,7 @@
         <v>130</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D58" s="9">
         <v>1</v>
@@ -3838,11 +3838,11 @@
         <v>2</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="F114" s="9"/>
       <c r="G114" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3859,11 +3859,11 @@
         <v>0</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="F115" s="9"/>
       <c r="G115" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -3880,11 +3880,11 @@
         <v>1</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="F116" s="9"/>
       <c r="G116" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -3892,7 +3892,7 @@
         <v>0</v>
       </c>
       <c r="B117" s="27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C117" s="9" t="s">
         <v>7</v>
@@ -3901,11 +3901,11 @@
         <v>2</v>
       </c>
       <c r="E117" s="28" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F117" s="9"/>
       <c r="G117" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -3913,20 +3913,20 @@
         <v>0</v>
       </c>
       <c r="B118" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="C118" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D118" s="22">
+        <v>0</v>
+      </c>
+      <c r="E118" s="28" t="s">
         <v>281</v>
-      </c>
-      <c r="C118" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D118" s="22">
-        <v>0</v>
-      </c>
-      <c r="E118" s="28" t="s">
-        <v>282</v>
       </c>
       <c r="F118" s="9"/>
       <c r="G118" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -4016,8 +4016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:A47"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4078,7 +4078,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>185</v>
@@ -4744,7 +4744,7 @@
         <v>0</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>7</v>
@@ -4762,7 +4762,7 @@
         <v>0</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>33</v>
@@ -4780,17 +4780,17 @@
         <v>0</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
change icons some quest
Former-commit-id: 756cf9aa354489c01bc7924b8909b768b4743d3a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tournaments" sheetId="2" r:id="rId1"/>
@@ -1273,7 +1273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1365,6 +1365,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1647,8 +1655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="G133" sqref="G133"/>
+    <sheetView topLeftCell="F128" workbookViewId="0">
+      <selection activeCell="G139" sqref="G139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4979,8 +4987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:F54"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5774,21 +5782,21 @@
         <v>293</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" s="31" t="s">
+    <row r="46" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="42" t="s">
         <v>294</v>
       </c>
-      <c r="C46" s="30" t="s">
+      <c r="C46" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D46" s="31" t="s">
+      <c r="D46" s="42" t="s">
         <v>295</v>
       </c>
-      <c r="E46" s="30"/>
-      <c r="F46" s="32" t="s">
+      <c r="E46" s="41"/>
+      <c r="F46" s="43" t="s">
         <v>296</v>
       </c>
     </row>
@@ -5860,7 +5868,7 @@
         <v>216</v>
       </c>
       <c r="E50" s="9"/>
-      <c r="F50" s="12" t="s">
+      <c r="F50" s="36" t="s">
         <v>43</v>
       </c>
     </row>
@@ -5878,61 +5886,61 @@
         <v>281</v>
       </c>
       <c r="E51" s="9"/>
-      <c r="F51" s="12" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="33" t="s">
+      <c r="F51" s="36" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="44" t="s">
         <v>303</v>
       </c>
-      <c r="C52" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="33" t="s">
+      <c r="C52" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="44" t="s">
         <v>304</v>
       </c>
-      <c r="E52" s="30"/>
-      <c r="F52" s="32" t="s">
+      <c r="E52" s="41"/>
+      <c r="F52" s="43" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="53" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="44" t="s">
         <v>306</v>
       </c>
-      <c r="C53" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="7" t="s">
+      <c r="C53" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="42" t="s">
         <v>307</v>
       </c>
-      <c r="E53" s="30"/>
-      <c r="F53" s="32" t="s">
+      <c r="E53" s="41"/>
+      <c r="F53" s="43" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B54" t="s">
+    <row r="54" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="44" t="s">
         <v>350</v>
       </c>
-      <c r="C54" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" s="7" t="s">
+      <c r="C54" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="42" t="s">
         <v>348</v>
       </c>
-      <c r="E54" s="30"/>
-      <c r="F54" s="32" t="s">
+      <c r="E54" s="41"/>
+      <c r="F54" s="43" t="s">
         <v>349</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed normal firerush tournament type number
Former-commit-id: e84ba3cb4afd9cbcdb321d6bcc5277499867105d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860"/>
   </bookViews>
   <sheets>
     <sheet name="tournaments" sheetId="2" r:id="rId1"/>
@@ -1655,8 +1655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G159"/>
   <sheetViews>
-    <sheetView topLeftCell="F128" workbookViewId="0">
-      <selection activeCell="G139" sqref="G139"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2194,7 +2194,7 @@
         <v>6</v>
       </c>
       <c r="D26" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
@@ -4987,7 +4987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed tournament type number fidh, present, candy
Former-commit-id: a666ad9844960d7034d99ab7a492d91320fecf34
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -1655,8 +1655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="B153" sqref="B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2213,7 +2213,7 @@
         <v>6</v>
       </c>
       <c r="D27" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
@@ -2232,7 +2232,7 @@
         <v>6</v>
       </c>
       <c r="D28" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
@@ -2274,7 +2274,7 @@
         <v>7</v>
       </c>
       <c r="D30" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>92</v>
@@ -2297,7 +2297,7 @@
         <v>7</v>
       </c>
       <c r="D31" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>92</v>
@@ -4398,7 +4398,7 @@
         <v>7</v>
       </c>
       <c r="D130" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E130" s="7" t="s">
         <v>195</v>
@@ -4419,7 +4419,7 @@
         <v>7</v>
       </c>
       <c r="D131" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E131" s="7" t="s">
         <v>195</v>
@@ -4440,7 +4440,7 @@
         <v>7</v>
       </c>
       <c r="D132" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E132" s="7" t="s">
         <v>195</v>

</xml_diff>

<commit_message>
fix name icon alien
Former-commit-id: 02cede32b4e64d2fc524e2638e7ba31a47f29f15
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="363">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -1113,6 +1113,9 @@
   </si>
   <si>
     <t>alien_mask</t>
+  </si>
+  <si>
+    <t>icon_ufo_mask_humanoids</t>
   </si>
 </sst>
 </file>
@@ -1685,8 +1688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="B162" sqref="B162"/>
+    <sheetView tabSelected="1" topLeftCell="C142" workbookViewId="0">
+      <selection activeCell="G162" sqref="G162:G164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5106,7 +5109,7 @@
         <v>361</v>
       </c>
       <c r="G162" s="11" t="s">
-        <v>41</v>
+        <v>362</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
@@ -5127,7 +5130,7 @@
       </c>
       <c r="F163" s="9"/>
       <c r="G163" s="11" t="s">
-        <v>41</v>
+        <v>362</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -5148,7 +5151,7 @@
       </c>
       <c r="F164" s="9"/>
       <c r="G164" s="11" t="s">
-        <v>41</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tournament and quest werewolf and creatures halloween
Former-commit-id: ed4120262202920807b433fb2b3851c935c4cfdf
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tournaments" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="370">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -377,9 +377,6 @@
     <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_HUMANS</t>
   </si>
   <si>
-    <t>RichMan;BoatFisher;BakerWoman;BadFarmer;Soldier;Archer01;Archer02;ShieldMan;DrunkenMan;Catapulter;Villager01;Villager02</t>
-  </si>
-  <si>
     <t>Humans</t>
   </si>
   <si>
@@ -1116,6 +1113,30 @@
   </si>
   <si>
     <t>icon_ufo_mask_humanoids</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_HALLOWEEN_CREATURES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_HALLOWEEN_CREATURES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_HALLOWEEN_CREATURES</t>
+  </si>
+  <si>
+    <t>Villager03</t>
+  </si>
+  <si>
+    <t>Witch;BadWitch;GoodWitch;GoodWitch02;RichMan;BoatFisher;BakerWoman;Villager01;Villager02;Villager03;Villager04</t>
+  </si>
+  <si>
+    <t>RichMan;BoatFisher;BakerWoman;BadFarmer;Soldier;Archer01;Archer02;ShieldMan;DrunkenMan;Catapulter;Villager01;Villager02;Villager03;Villager04;TubeMan;VillagerGirl</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_HALLOWEEN_CREATURES</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_WEREWOLF</t>
   </si>
 </sst>
 </file>
@@ -1686,10 +1707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G164"/>
+  <dimension ref="A1:G167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C142" workbookViewId="0">
-      <selection activeCell="G162" sqref="G162:G164"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="E167" sqref="E167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1962,7 +1983,7 @@
         <v>70</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D14" s="9">
         <v>0</v>
@@ -2125,7 +2146,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="11" t="s">
@@ -2146,7 +2167,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="11" t="s">
@@ -2167,7 +2188,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="11" t="s">
@@ -2557,7 +2578,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="11" t="s">
@@ -2578,7 +2599,7 @@
         <v>2</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="11" t="s">
@@ -2599,7 +2620,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="11" t="s">
@@ -2620,10 +2641,10 @@
         <v>0</v>
       </c>
       <c r="E44" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="F44" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="G44" s="11" t="s">
         <v>25</v>
@@ -2643,10 +2664,10 @@
         <v>2</v>
       </c>
       <c r="E45" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="F45" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="G45" s="11" t="s">
         <v>25</v>
@@ -2666,10 +2687,10 @@
         <v>1</v>
       </c>
       <c r="E46" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="F46" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="F46" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="G46" s="11" t="s">
         <v>25</v>
@@ -2680,7 +2701,7 @@
         <v>0</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>3</v>
@@ -2701,7 +2722,7 @@
         <v>0</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>3</v>
@@ -2722,7 +2743,7 @@
         <v>0</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>3</v>
@@ -2743,7 +2764,7 @@
         <v>0</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>7</v>
@@ -2752,7 +2773,7 @@
         <v>0</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F50" s="9"/>
       <c r="G50" s="11" t="s">
@@ -2764,7 +2785,7 @@
         <v>0</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>7</v>
@@ -2773,7 +2794,7 @@
         <v>2</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F51" s="9"/>
       <c r="G51" s="11" t="s">
@@ -2785,7 +2806,7 @@
         <v>0</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>7</v>
@@ -2794,7 +2815,7 @@
         <v>1</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F52" s="9"/>
       <c r="G52" s="11" t="s">
@@ -2806,10 +2827,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D53" s="9">
         <v>0</v>
@@ -2825,10 +2846,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D54" s="9">
         <v>2</v>
@@ -2844,10 +2865,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D55" s="9">
         <v>1</v>
@@ -2863,10 +2884,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D56" s="9">
         <v>0</v>
@@ -2882,10 +2903,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D57" s="9">
         <v>2</v>
@@ -2901,10 +2922,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D58" s="9">
         <v>1</v>
@@ -2920,7 +2941,7 @@
         <v>0</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>33</v>
@@ -2929,7 +2950,7 @@
         <v>0</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="11" t="s">
@@ -2941,7 +2962,7 @@
         <v>0</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>33</v>
@@ -2950,7 +2971,7 @@
         <v>2</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F60" s="9"/>
       <c r="G60" s="11" t="s">
@@ -2962,7 +2983,7 @@
         <v>0</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C61" s="9" t="s">
         <v>33</v>
@@ -2971,7 +2992,7 @@
         <v>1</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F61" s="9"/>
       <c r="G61" s="11" t="s">
@@ -2983,7 +3004,7 @@
         <v>0</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>7</v>
@@ -3004,7 +3025,7 @@
         <v>0</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C63" s="9" t="s">
         <v>7</v>
@@ -3025,7 +3046,7 @@
         <v>0</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>7</v>
@@ -3046,7 +3067,7 @@
         <v>0</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C65" s="9" t="s">
         <v>33</v>
@@ -3055,7 +3076,7 @@
         <v>0</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F65" s="9"/>
       <c r="G65" s="11" t="s">
@@ -3067,7 +3088,7 @@
         <v>0</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>33</v>
@@ -3076,7 +3097,7 @@
         <v>2</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F66" s="9"/>
       <c r="G66" s="11" t="s">
@@ -3088,7 +3109,7 @@
         <v>0</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C67" s="9" t="s">
         <v>33</v>
@@ -3097,7 +3118,7 @@
         <v>1</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F67" s="9"/>
       <c r="G67" s="11" t="s">
@@ -3109,7 +3130,7 @@
         <v>0</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C68" s="9" t="s">
         <v>7</v>
@@ -3118,10 +3139,10 @@
         <v>0</v>
       </c>
       <c r="E68" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F68" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="F68" s="9" t="s">
-        <v>144</v>
       </c>
       <c r="G68" s="11" t="s">
         <v>42</v>
@@ -3132,7 +3153,7 @@
         <v>0</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C69" s="9" t="s">
         <v>7</v>
@@ -3141,10 +3162,10 @@
         <v>2</v>
       </c>
       <c r="E69" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F69" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="F69" s="9" t="s">
-        <v>144</v>
       </c>
       <c r="G69" s="11" t="s">
         <v>42</v>
@@ -3155,7 +3176,7 @@
         <v>0</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>7</v>
@@ -3164,10 +3185,10 @@
         <v>1</v>
       </c>
       <c r="E70" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F70" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="F70" s="9" t="s">
-        <v>144</v>
       </c>
       <c r="G70" s="11" t="s">
         <v>42</v>
@@ -3178,7 +3199,7 @@
         <v>0</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C71" s="9" t="s">
         <v>30</v>
@@ -3187,11 +3208,11 @@
         <v>0</v>
       </c>
       <c r="E71" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F71" s="9"/>
       <c r="G71" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3199,7 +3220,7 @@
         <v>0</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C72" s="9" t="s">
         <v>30</v>
@@ -3208,11 +3229,11 @@
         <v>2</v>
       </c>
       <c r="E72" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F72" s="9"/>
       <c r="G72" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3220,7 +3241,7 @@
         <v>0</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>30</v>
@@ -3229,11 +3250,11 @@
         <v>1</v>
       </c>
       <c r="E73" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F73" s="9"/>
       <c r="G73" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3241,7 +3262,7 @@
         <v>0</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>32</v>
@@ -3250,11 +3271,11 @@
         <v>0</v>
       </c>
       <c r="E74" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F74" s="9"/>
       <c r="G74" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3262,7 +3283,7 @@
         <v>0</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C75" s="9" t="s">
         <v>32</v>
@@ -3271,11 +3292,11 @@
         <v>2</v>
       </c>
       <c r="E75" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F75" s="9"/>
       <c r="G75" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -3283,7 +3304,7 @@
         <v>0</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>32</v>
@@ -3292,11 +3313,11 @@
         <v>1</v>
       </c>
       <c r="E76" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F76" s="9"/>
       <c r="G76" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -3304,7 +3325,7 @@
         <v>0</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C77" s="12" t="s">
         <v>46</v>
@@ -3342,7 +3363,7 @@
         <v>0</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>46</v>
@@ -3361,7 +3382,7 @@
         <v>0</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C80" s="12" t="s">
         <v>48</v>
@@ -3399,7 +3420,7 @@
         <v>0</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C82" s="9" t="s">
         <v>7</v>
@@ -3408,13 +3429,13 @@
         <v>0</v>
       </c>
       <c r="E82" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="G82" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="F82" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G82" s="9" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3422,7 +3443,7 @@
         <v>0</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>7</v>
@@ -3431,13 +3452,13 @@
         <v>2</v>
       </c>
       <c r="E83" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="G83" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="F83" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G83" s="9" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3445,7 +3466,7 @@
         <v>0</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C84" s="9" t="s">
         <v>7</v>
@@ -3454,13 +3475,13 @@
         <v>1</v>
       </c>
       <c r="E84" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="G84" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G84" s="9" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3468,7 +3489,7 @@
         <v>0</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C85" s="9" t="s">
         <v>7</v>
@@ -3489,7 +3510,7 @@
         <v>0</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C86" s="9" t="s">
         <v>7</v>
@@ -3510,7 +3531,7 @@
         <v>0</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C87" s="9" t="s">
         <v>7</v>
@@ -3531,7 +3552,7 @@
         <v>0</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C88" s="9" t="s">
         <v>7</v>
@@ -3540,10 +3561,10 @@
         <v>0</v>
       </c>
       <c r="E88" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F88" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="F88" s="9" t="s">
-        <v>170</v>
       </c>
       <c r="G88" s="11" t="s">
         <v>39</v>
@@ -3554,7 +3575,7 @@
         <v>0</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C89" s="9" t="s">
         <v>7</v>
@@ -3563,10 +3584,10 @@
         <v>2</v>
       </c>
       <c r="E89" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F89" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="F89" s="9" t="s">
-        <v>170</v>
       </c>
       <c r="G89" s="11" t="s">
         <v>39</v>
@@ -3577,7 +3598,7 @@
         <v>0</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C90" s="9" t="s">
         <v>7</v>
@@ -3586,10 +3607,10 @@
         <v>1</v>
       </c>
       <c r="E90" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F90" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="F90" s="9" t="s">
-        <v>170</v>
       </c>
       <c r="G90" s="11" t="s">
         <v>39</v>
@@ -3600,7 +3621,7 @@
         <v>0</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C91" s="9" t="s">
         <v>7</v>
@@ -3609,7 +3630,7 @@
         <v>0</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F91" s="9"/>
       <c r="G91" s="11" t="s">
@@ -3621,7 +3642,7 @@
         <v>0</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C92" s="9" t="s">
         <v>7</v>
@@ -3630,7 +3651,7 @@
         <v>2</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F92" s="9"/>
       <c r="G92" s="11" t="s">
@@ -3642,7 +3663,7 @@
         <v>0</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C93" s="9" t="s">
         <v>7</v>
@@ -3651,7 +3672,7 @@
         <v>1</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F93" s="9"/>
       <c r="G93" s="11" t="s">
@@ -3663,7 +3684,7 @@
         <v>0</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C94" s="9" t="s">
         <v>33</v>
@@ -3672,7 +3693,7 @@
         <v>0</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F94" s="9"/>
       <c r="G94" s="11" t="s">
@@ -3684,7 +3705,7 @@
         <v>0</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C95" s="9" t="s">
         <v>33</v>
@@ -3693,7 +3714,7 @@
         <v>2</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F95" s="9"/>
       <c r="G95" s="11" t="s">
@@ -3705,7 +3726,7 @@
         <v>0</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C96" s="9" t="s">
         <v>33</v>
@@ -3714,7 +3735,7 @@
         <v>1</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F96" s="9"/>
       <c r="G96" s="11" t="s">
@@ -3726,20 +3747,20 @@
         <v>0</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D97" s="9">
         <v>0</v>
       </c>
       <c r="E97" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F97" s="9"/>
       <c r="G97" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3747,20 +3768,20 @@
         <v>0</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D98" s="9">
         <v>2</v>
       </c>
       <c r="E98" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F98" s="9"/>
       <c r="G98" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3768,20 +3789,20 @@
         <v>0</v>
       </c>
       <c r="B99" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C99" s="9" t="s">
         <v>181</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>182</v>
       </c>
       <c r="D99" s="9">
         <v>1</v>
       </c>
       <c r="E99" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F99" s="9"/>
       <c r="G99" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3789,7 +3810,7 @@
         <v>0</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C100" s="9" t="s">
         <v>7</v>
@@ -3798,11 +3819,11 @@
         <v>0</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F100" s="9"/>
       <c r="G100" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3810,7 +3831,7 @@
         <v>0</v>
       </c>
       <c r="B101" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C101" s="9" t="s">
         <v>7</v>
@@ -3819,11 +3840,11 @@
         <v>2</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F101" s="9"/>
       <c r="G101" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3831,7 +3852,7 @@
         <v>0</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C102" s="9" t="s">
         <v>7</v>
@@ -3840,11 +3861,11 @@
         <v>1</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F102" s="9"/>
       <c r="G102" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3852,7 +3873,7 @@
         <v>0</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C103" s="9" t="s">
         <v>7</v>
@@ -3861,11 +3882,11 @@
         <v>0</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F103" s="9"/>
       <c r="G103" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3873,7 +3894,7 @@
         <v>0</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C104" s="9" t="s">
         <v>7</v>
@@ -3882,11 +3903,11 @@
         <v>2</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F104" s="9"/>
       <c r="G104" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3894,7 +3915,7 @@
         <v>0</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C105" s="9" t="s">
         <v>7</v>
@@ -3903,11 +3924,11 @@
         <v>1</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F105" s="9"/>
       <c r="G105" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3915,7 +3936,7 @@
         <v>0</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C106" s="9" t="s">
         <v>33</v>
@@ -3924,13 +3945,13 @@
         <v>0</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F106" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="G106" s="12" t="s">
         <v>247</v>
-      </c>
-      <c r="G106" s="12" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3938,7 +3959,7 @@
         <v>0</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C107" s="9" t="s">
         <v>33</v>
@@ -3947,13 +3968,13 @@
         <v>2</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F107" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="G107" s="12" t="s">
         <v>247</v>
-      </c>
-      <c r="G107" s="12" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3961,7 +3982,7 @@
         <v>0</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C108" s="9" t="s">
         <v>33</v>
@@ -3970,13 +3991,13 @@
         <v>1</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F108" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="G108" s="12" t="s">
         <v>247</v>
-      </c>
-      <c r="G108" s="12" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -3984,7 +4005,7 @@
         <v>0</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C109" s="9" t="s">
         <v>33</v>
@@ -3993,11 +4014,11 @@
         <v>0</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F109" s="9"/>
       <c r="G109" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -4005,7 +4026,7 @@
         <v>0</v>
       </c>
       <c r="B110" s="23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C110" s="9" t="s">
         <v>33</v>
@@ -4014,11 +4035,11 @@
         <v>2</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F110" s="9"/>
       <c r="G110" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -4026,7 +4047,7 @@
         <v>0</v>
       </c>
       <c r="B111" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C111" s="9" t="s">
         <v>7</v>
@@ -4035,11 +4056,11 @@
         <v>2</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F111" s="9"/>
       <c r="G111" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -4047,7 +4068,7 @@
         <v>0</v>
       </c>
       <c r="B112" s="25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C112" s="9" t="s">
         <v>7</v>
@@ -4056,11 +4077,11 @@
         <v>0</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F112" s="9"/>
       <c r="G112" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -4068,7 +4089,7 @@
         <v>0</v>
       </c>
       <c r="B113" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C113" s="9" t="s">
         <v>7</v>
@@ -4077,11 +4098,11 @@
         <v>1</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F113" s="9"/>
       <c r="G113" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -4089,7 +4110,7 @@
         <v>0</v>
       </c>
       <c r="B114" s="25" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C114" s="9" t="s">
         <v>7</v>
@@ -4098,11 +4119,11 @@
         <v>2</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F114" s="9"/>
       <c r="G114" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -4110,7 +4131,7 @@
         <v>0</v>
       </c>
       <c r="B115" s="25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C115" s="9" t="s">
         <v>7</v>
@@ -4119,11 +4140,11 @@
         <v>0</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F115" s="9"/>
       <c r="G115" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -4131,7 +4152,7 @@
         <v>0</v>
       </c>
       <c r="B116" s="26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C116" s="9" t="s">
         <v>7</v>
@@ -4140,11 +4161,11 @@
         <v>1</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F116" s="9"/>
       <c r="G116" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -4152,7 +4173,7 @@
         <v>0</v>
       </c>
       <c r="B117" s="27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C117" s="9" t="s">
         <v>7</v>
@@ -4161,11 +4182,11 @@
         <v>2</v>
       </c>
       <c r="E117" s="28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F117" s="9"/>
       <c r="G117" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -4173,20 +4194,20 @@
         <v>0</v>
       </c>
       <c r="B118" s="27" t="s">
+        <v>279</v>
+      </c>
+      <c r="C118" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D118" s="22">
+        <v>0</v>
+      </c>
+      <c r="E118" s="28" t="s">
         <v>280</v>
-      </c>
-      <c r="C118" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D118" s="22">
-        <v>0</v>
-      </c>
-      <c r="E118" s="28" t="s">
-        <v>281</v>
       </c>
       <c r="F118" s="9"/>
       <c r="G118" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="119" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -4194,7 +4215,7 @@
         <v>0</v>
       </c>
       <c r="B119" s="35" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C119" s="30" t="s">
         <v>7</v>
@@ -4203,11 +4224,11 @@
         <v>0</v>
       </c>
       <c r="E119" s="31" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F119" s="30"/>
       <c r="G119" s="30" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -4215,7 +4236,7 @@
         <v>0</v>
       </c>
       <c r="B120" s="24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C120" s="9" t="s">
         <v>7</v>
@@ -4224,11 +4245,11 @@
         <v>2</v>
       </c>
       <c r="E120" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F120" s="9"/>
       <c r="G120" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -4236,7 +4257,7 @@
         <v>0</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C121" s="9" t="s">
         <v>7</v>
@@ -4245,11 +4266,11 @@
         <v>1</v>
       </c>
       <c r="E121" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F121" s="9"/>
       <c r="G121" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -4257,7 +4278,7 @@
         <v>0</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C122" s="9" t="s">
         <v>7</v>
@@ -4266,11 +4287,11 @@
         <v>0</v>
       </c>
       <c r="E122" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F122" s="9"/>
       <c r="G122" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -4278,7 +4299,7 @@
         <v>0</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C123" s="9" t="s">
         <v>7</v>
@@ -4287,11 +4308,11 @@
         <v>2</v>
       </c>
       <c r="E123" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F123" s="9"/>
       <c r="G123" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -4299,7 +4320,7 @@
         <v>0</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C124" s="9" t="s">
         <v>7</v>
@@ -4308,11 +4329,11 @@
         <v>1</v>
       </c>
       <c r="E124" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F124" s="9"/>
       <c r="G124" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -4320,7 +4341,7 @@
         <v>0</v>
       </c>
       <c r="B125" s="13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C125" s="9" t="s">
         <v>7</v>
@@ -4329,11 +4350,11 @@
         <v>0</v>
       </c>
       <c r="E125" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F125" s="9"/>
       <c r="G125" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -4341,7 +4362,7 @@
         <v>0</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C126" s="9" t="s">
         <v>7</v>
@@ -4350,11 +4371,11 @@
         <v>2</v>
       </c>
       <c r="E126" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F126" s="9"/>
       <c r="G126" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -4362,7 +4383,7 @@
         <v>0</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C127" s="9" t="s">
         <v>7</v>
@@ -4371,11 +4392,11 @@
         <v>1</v>
       </c>
       <c r="E127" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F127" s="9"/>
       <c r="G127" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4383,20 +4404,20 @@
         <v>0</v>
       </c>
       <c r="B128" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="C128" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D128" s="9">
+        <v>0</v>
+      </c>
+      <c r="E128" s="7" t="s">
         <v>318</v>
-      </c>
-      <c r="C128" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D128" s="9">
-        <v>0</v>
-      </c>
-      <c r="E128" s="7" t="s">
-        <v>319</v>
       </c>
       <c r="F128" s="9"/>
       <c r="G128" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -4404,7 +4425,7 @@
         <v>0</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C129" s="9" t="s">
         <v>7</v>
@@ -4413,11 +4434,11 @@
         <v>2</v>
       </c>
       <c r="E129" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F129" s="9"/>
       <c r="G129" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -4425,7 +4446,7 @@
         <v>0</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C130" s="9" t="s">
         <v>7</v>
@@ -4434,11 +4455,11 @@
         <v>0</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F130" s="9"/>
       <c r="G130" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -4446,7 +4467,7 @@
         <v>0</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C131" s="9" t="s">
         <v>7</v>
@@ -4455,11 +4476,11 @@
         <v>2</v>
       </c>
       <c r="E131" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F131" s="9"/>
       <c r="G131" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -4467,7 +4488,7 @@
         <v>0</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C132" s="9" t="s">
         <v>7</v>
@@ -4476,11 +4497,11 @@
         <v>1</v>
       </c>
       <c r="E132" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F132" s="9"/>
       <c r="G132" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="133" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4488,7 +4509,7 @@
         <v>0</v>
       </c>
       <c r="B133" s="37" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C133" s="36" t="s">
         <v>7</v>
@@ -4497,11 +4518,11 @@
         <v>1</v>
       </c>
       <c r="E133" s="37" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F133" s="36"/>
       <c r="G133" s="36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="134" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4509,7 +4530,7 @@
         <v>0</v>
       </c>
       <c r="B134" s="37" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C134" s="36" t="s">
         <v>7</v>
@@ -4518,11 +4539,11 @@
         <v>2</v>
       </c>
       <c r="E134" s="37" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F134" s="36"/>
       <c r="G134" s="36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="135" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4530,7 +4551,7 @@
         <v>0</v>
       </c>
       <c r="B135" s="37" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C135" s="36" t="s">
         <v>7</v>
@@ -4539,11 +4560,11 @@
         <v>1</v>
       </c>
       <c r="E135" s="37" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F135" s="36"/>
       <c r="G135" s="36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -4551,7 +4572,7 @@
         <v>0</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C136" s="9" t="s">
         <v>7</v>
@@ -4560,11 +4581,11 @@
         <v>0</v>
       </c>
       <c r="E136" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F136" s="9"/>
       <c r="G136" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -4572,7 +4593,7 @@
         <v>0</v>
       </c>
       <c r="B137" s="13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C137" s="9" t="s">
         <v>7</v>
@@ -4581,11 +4602,11 @@
         <v>2</v>
       </c>
       <c r="E137" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F137" s="9"/>
       <c r="G137" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -4593,7 +4614,7 @@
         <v>0</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C138" s="9" t="s">
         <v>7</v>
@@ -4602,11 +4623,11 @@
         <v>1</v>
       </c>
       <c r="E138" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F138" s="9"/>
       <c r="G138" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="139" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4614,7 +4635,7 @@
         <v>0</v>
       </c>
       <c r="B139" s="37" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C139" s="36" t="s">
         <v>46</v>
@@ -4623,7 +4644,7 @@
         <v>2</v>
       </c>
       <c r="E139" s="37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F139" s="36"/>
       <c r="G139" s="36" t="s">
@@ -4635,7 +4656,7 @@
         <v>0</v>
       </c>
       <c r="B140" s="37" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C140" s="36" t="s">
         <v>46</v>
@@ -4644,7 +4665,7 @@
         <v>0</v>
       </c>
       <c r="E140" s="37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F140" s="36"/>
       <c r="G140" s="36" t="s">
@@ -4656,7 +4677,7 @@
         <v>0</v>
       </c>
       <c r="B141" s="37" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C141" s="36" t="s">
         <v>46</v>
@@ -4665,7 +4686,7 @@
         <v>2</v>
       </c>
       <c r="E141" s="37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F141" s="36"/>
       <c r="G141" s="36" t="s">
@@ -4677,7 +4698,7 @@
         <v>0</v>
       </c>
       <c r="B142" s="37" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C142" s="36" t="s">
         <v>48</v>
@@ -4686,7 +4707,7 @@
         <v>2</v>
       </c>
       <c r="E142" s="37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F142" s="36"/>
       <c r="G142" s="36" t="s">
@@ -4698,7 +4719,7 @@
         <v>0</v>
       </c>
       <c r="B143" s="37" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C143" s="36" t="s">
         <v>46</v>
@@ -4707,7 +4728,7 @@
         <v>0</v>
       </c>
       <c r="E143" s="37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F143" s="36"/>
       <c r="G143" s="36" t="s">
@@ -4719,7 +4740,7 @@
         <v>0</v>
       </c>
       <c r="B144" s="37" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C144" s="36" t="s">
         <v>46</v>
@@ -4728,7 +4749,7 @@
         <v>1</v>
       </c>
       <c r="E144" s="37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F144" s="36"/>
       <c r="G144" s="36" t="s">
@@ -4740,7 +4761,7 @@
         <v>0</v>
       </c>
       <c r="B145" s="37" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C145" s="36" t="s">
         <v>48</v>
@@ -4749,7 +4770,7 @@
         <v>0</v>
       </c>
       <c r="E145" s="37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F145" s="36"/>
       <c r="G145" s="36" t="s">
@@ -4761,7 +4782,7 @@
         <v>0</v>
       </c>
       <c r="B146" s="37" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C146" s="36" t="s">
         <v>7</v>
@@ -4770,11 +4791,11 @@
         <v>2</v>
       </c>
       <c r="E146" s="37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F146" s="36"/>
       <c r="G146" s="36" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="147" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4782,7 +4803,7 @@
         <v>0</v>
       </c>
       <c r="B147" s="37" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C147" s="36" t="s">
         <v>7</v>
@@ -4791,11 +4812,11 @@
         <v>0</v>
       </c>
       <c r="E147" s="37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F147" s="36"/>
       <c r="G147" s="36" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="148" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4803,7 +4824,7 @@
         <v>0</v>
       </c>
       <c r="B148" s="37" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C148" s="36" t="s">
         <v>46</v>
@@ -4812,11 +4833,11 @@
         <v>2</v>
       </c>
       <c r="E148" s="37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F148" s="36"/>
       <c r="G148" s="36" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="149" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4824,7 +4845,7 @@
         <v>0</v>
       </c>
       <c r="B149" s="37" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C149" s="36" t="s">
         <v>48</v>
@@ -4833,11 +4854,11 @@
         <v>2</v>
       </c>
       <c r="E149" s="37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F149" s="36"/>
       <c r="G149" s="36" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="150" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4845,7 +4866,7 @@
         <v>0</v>
       </c>
       <c r="B150" s="37" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C150" s="36" t="s">
         <v>46</v>
@@ -4854,11 +4875,11 @@
         <v>0</v>
       </c>
       <c r="E150" s="37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F150" s="36"/>
       <c r="G150" s="36" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="151" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4866,7 +4887,7 @@
         <v>0</v>
       </c>
       <c r="B151" s="37" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C151" s="36" t="s">
         <v>46</v>
@@ -4875,11 +4896,11 @@
         <v>1</v>
       </c>
       <c r="E151" s="37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F151" s="36"/>
       <c r="G151" s="36" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="152" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4887,7 +4908,7 @@
         <v>0</v>
       </c>
       <c r="B152" s="37" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C152" s="36" t="s">
         <v>48</v>
@@ -4896,11 +4917,11 @@
         <v>0</v>
       </c>
       <c r="E152" s="37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F152" s="36"/>
       <c r="G152" s="36" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="153" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4908,7 +4929,7 @@
         <v>0</v>
       </c>
       <c r="B153" s="39" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C153" s="36" t="s">
         <v>7</v>
@@ -4917,11 +4938,11 @@
         <v>0</v>
       </c>
       <c r="E153" s="37" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F153" s="36"/>
       <c r="G153" s="36" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="154" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4929,7 +4950,7 @@
         <v>0</v>
       </c>
       <c r="B154" s="40" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C154" s="36" t="s">
         <v>7</v>
@@ -4938,11 +4959,11 @@
         <v>2</v>
       </c>
       <c r="E154" s="37" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F154" s="36"/>
       <c r="G154" s="36" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="155" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4950,7 +4971,7 @@
         <v>0</v>
       </c>
       <c r="B155" s="37" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C155" s="36" t="s">
         <v>7</v>
@@ -4959,11 +4980,11 @@
         <v>1</v>
       </c>
       <c r="E155" s="37" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F155" s="36"/>
       <c r="G155" s="36" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -4971,7 +4992,7 @@
         <v>0</v>
       </c>
       <c r="B156" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C156" s="9" t="s">
         <v>7</v>
@@ -4980,11 +5001,11 @@
         <v>0</v>
       </c>
       <c r="E156" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F156" s="9"/>
       <c r="G156" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -4992,7 +5013,7 @@
         <v>0</v>
       </c>
       <c r="B157" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C157" s="9" t="s">
         <v>7</v>
@@ -5001,11 +5022,11 @@
         <v>2</v>
       </c>
       <c r="E157" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F157" s="9"/>
       <c r="G157" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -5013,7 +5034,7 @@
         <v>0</v>
       </c>
       <c r="B158" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C158" s="9" t="s">
         <v>7</v>
@@ -5022,11 +5043,11 @@
         <v>1</v>
       </c>
       <c r="E158" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F158" s="9"/>
       <c r="G158" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -5034,7 +5055,7 @@
         <v>0</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C159" s="9" t="s">
         <v>7</v>
@@ -5043,11 +5064,11 @@
         <v>0</v>
       </c>
       <c r="E159" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F159" s="9"/>
       <c r="G159" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -5055,7 +5076,7 @@
         <v>0</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C160" s="9" t="s">
         <v>7</v>
@@ -5064,11 +5085,11 @@
         <v>2</v>
       </c>
       <c r="E160" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F160" s="9"/>
       <c r="G160" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -5076,7 +5097,7 @@
         <v>0</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C161" s="9" t="s">
         <v>7</v>
@@ -5085,11 +5106,11 @@
         <v>1</v>
       </c>
       <c r="E161" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F161" s="9"/>
       <c r="G161" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -5097,7 +5118,7 @@
         <v>0</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C162" s="9" t="s">
         <v>33</v>
@@ -5106,10 +5127,10 @@
         <v>2</v>
       </c>
       <c r="E162" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="G162" s="11" t="s">
         <v>361</v>
-      </c>
-      <c r="G162" s="11" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
@@ -5117,7 +5138,7 @@
         <v>0</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C163" s="9" t="s">
         <v>33</v>
@@ -5126,11 +5147,11 @@
         <v>0</v>
       </c>
       <c r="E163" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F163" s="9"/>
       <c r="G163" s="11" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -5138,7 +5159,7 @@
         <v>0</v>
       </c>
       <c r="B164" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C164" s="9" t="s">
         <v>33</v>
@@ -5147,11 +5168,73 @@
         <v>1</v>
       </c>
       <c r="E164" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F164" s="9"/>
       <c r="G164" s="11" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B165" s="13" t="s">
         <v>362</v>
+      </c>
+      <c r="C165" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D165" s="9">
+        <v>2</v>
+      </c>
+      <c r="E165" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="G165" s="12" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B166" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="C166" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D166" s="9">
+        <v>0</v>
+      </c>
+      <c r="E166" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="F166" s="9"/>
+      <c r="G166" s="12" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B167" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="C167" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D167" s="9">
+        <v>1</v>
+      </c>
+      <c r="E167" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="F167" s="9"/>
+      <c r="G167" s="12" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -5162,10 +5245,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:F6"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5181,7 +5264,7 @@
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -5197,7 +5280,7 @@
     </row>
     <row r="4" spans="1:6" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -5220,19 +5303,19 @@
         <v>0</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -5240,17 +5323,17 @@
         <v>0</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -5258,17 +5341,17 @@
         <v>0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -5276,17 +5359,17 @@
         <v>0</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -5294,17 +5377,17 @@
         <v>0</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -5312,13 +5395,13 @@
         <v>0</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="12" t="s">
@@ -5330,17 +5413,17 @@
         <v>0</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -5348,7 +5431,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>29</v>
@@ -5368,7 +5451,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>2</v>
@@ -5384,17 +5467,17 @@
         <v>0</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -5402,7 +5485,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>4</v>
@@ -5418,7 +5501,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>3</v>
@@ -5436,7 +5519,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>46</v>
@@ -5452,7 +5535,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>7</v>
@@ -5472,7 +5555,7 @@
         <v>0</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>5</v>
@@ -5488,7 +5571,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>2</v>
@@ -5504,17 +5587,17 @@
         <v>0</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>207</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>208</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -5522,13 +5605,13 @@
         <v>0</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="12" t="s">
@@ -5540,7 +5623,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>6</v>
@@ -5556,13 +5639,13 @@
         <v>0</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="12" t="s">
@@ -5574,17 +5657,17 @@
         <v>0</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -5592,13 +5675,13 @@
         <v>0</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="12" t="s">
@@ -5610,13 +5693,13 @@
         <v>0</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>215</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>216</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="12" t="s">
@@ -5628,7 +5711,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>7</v>
@@ -5646,7 +5729,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>7</v>
@@ -5664,17 +5747,17 @@
         <v>0</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -5682,7 +5765,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>7</v>
@@ -5702,7 +5785,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>7</v>
@@ -5722,7 +5805,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>7</v>
@@ -5742,7 +5825,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>7</v>
@@ -5762,7 +5845,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>7</v>
@@ -5774,7 +5857,7 @@
         <v>108</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -5782,7 +5865,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>7</v>
@@ -5800,19 +5883,19 @@
         <v>0</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D37" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="F37" s="12" t="s">
         <v>160</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -5820,16 +5903,16 @@
         <v>0</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D38" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="E38" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>25</v>
@@ -5840,7 +5923,7 @@
         <v>0</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>7</v>
@@ -5848,7 +5931,7 @@
       <c r="D39" s="16"/>
       <c r="E39" s="14"/>
       <c r="F39" s="17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -5856,17 +5939,17 @@
         <v>0</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E40" s="18"/>
       <c r="F40" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -5874,17 +5957,17 @@
         <v>0</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -5892,17 +5975,17 @@
         <v>0</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -5910,17 +5993,17 @@
         <v>0</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -5928,17 +6011,17 @@
         <v>0</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -5946,17 +6029,17 @@
         <v>0</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -5964,17 +6047,17 @@
         <v>0</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C46" s="41" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="42" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E46" s="41"/>
       <c r="F46" s="43" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -5982,17 +6065,17 @@
         <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E47" s="9"/>
       <c r="F47" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -6000,17 +6083,17 @@
         <v>0</v>
       </c>
       <c r="B48" s="33" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C48" s="30" t="s">
         <v>3</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E48" s="30"/>
       <c r="F48" s="32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -6018,17 +6101,17 @@
         <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E49" s="9"/>
       <c r="F49" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -6036,13 +6119,13 @@
         <v>0</v>
       </c>
       <c r="B50" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E50" s="9"/>
       <c r="F50" s="36" t="s">
@@ -6054,17 +6137,17 @@
         <v>0</v>
       </c>
       <c r="B51" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E51" s="9"/>
       <c r="F51" s="36" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -6072,17 +6155,17 @@
         <v>0</v>
       </c>
       <c r="B52" s="44" t="s">
+        <v>302</v>
+      </c>
+      <c r="C52" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="44" t="s">
         <v>303</v>
-      </c>
-      <c r="C52" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="44" t="s">
-        <v>304</v>
       </c>
       <c r="E52" s="41"/>
       <c r="F52" s="43" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -6090,17 +6173,17 @@
         <v>0</v>
       </c>
       <c r="B53" s="44" t="s">
+        <v>305</v>
+      </c>
+      <c r="C53" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="42" t="s">
         <v>306</v>
-      </c>
-      <c r="C53" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="42" t="s">
-        <v>307</v>
       </c>
       <c r="E53" s="41"/>
       <c r="F53" s="43" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -6108,17 +6191,53 @@
         <v>0</v>
       </c>
       <c r="B54" s="44" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C54" s="41" t="s">
         <v>7</v>
       </c>
       <c r="D54" s="42" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E54" s="41"/>
       <c r="F54" s="43" t="s">
-        <v>349</v>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="E55" s="18"/>
+      <c r="F55" s="12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="E56" s="18"/>
+      <c r="F56" s="12" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added halloween creatures and werewolf quest and tou
Former-commit-id: 880b21c8f6070428ddb4348591020bf5c268691b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="22125" windowHeight="8475" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tournaments" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="371">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -1137,6 +1137,9 @@
   </si>
   <si>
     <t>TID_GLOBAL_EVENT_WEREWOLF</t>
+  </si>
+  <si>
+    <t>Witch;BadWitch;GoodWitch;GoodWitch02;RichMan;BoatFisher;BakerWoman;Villager01;Villager02;Villager03;Villager04;EnemyTier0;EnemyTier1;EnemyTier2;EnemyTier3;EnemyTier5;Ground_Zombie;Cow;Horse;Sheep;Troll;worker</t>
   </si>
 </sst>
 </file>
@@ -1709,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G167"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="E167" sqref="E167"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5247,8 +5250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6215,7 +6218,7 @@
         <v>7</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="E55" s="18"/>
       <c r="F55" s="12" t="s">

</xml_diff>

<commit_message>
fix some quest from collect to kill added cake tour
Former-commit-id: e4536dc6d22e9fde80786e59b47f868a4f62917c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="22125" windowHeight="8475"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="22125" windowHeight="8475" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tournaments" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="376">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -1152,6 +1152,9 @@
   </si>
   <si>
     <t>Canary01_Flock;Canary02_Flock;Canary03_Flock;Canary04_Flock;Hawk;OwlWhite;OwlBig;Vulture;Starling_Flock;CrowFlock;BatSmall_Flock;BatBig_Flock</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_EAT_NORMAL_BIRTHDAY_CAKE</t>
   </si>
 </sst>
 </file>
@@ -1722,10 +1725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G167"/>
+  <dimension ref="A1:G169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C138" sqref="C138:C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4652,8 +4655,8 @@
       <c r="B139" s="37" t="s">
         <v>329</v>
       </c>
-      <c r="C139" s="36" t="s">
-        <v>46</v>
+      <c r="C139" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="D139" s="36">
         <v>2</v>
@@ -4673,8 +4676,8 @@
       <c r="B140" s="37" t="s">
         <v>330</v>
       </c>
-      <c r="C140" s="36" t="s">
-        <v>46</v>
+      <c r="C140" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="D140" s="36">
         <v>0</v>
@@ -5250,6 +5253,48 @@
       <c r="F167" s="9"/>
       <c r="G167" s="12" t="s">
         <v>246</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B168" t="s">
+        <v>375</v>
+      </c>
+      <c r="C168" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D168" s="36">
+        <v>2</v>
+      </c>
+      <c r="E168" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="F168" s="36"/>
+      <c r="G168" s="36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B169" t="s">
+        <v>375</v>
+      </c>
+      <c r="C169" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D169" s="36">
+        <v>0</v>
+      </c>
+      <c r="E169" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="F169" s="36"/>
+      <c r="G169" s="36" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -5262,8 +5307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5321,7 +5366,7 @@
         <v>182</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>287</v>
@@ -5341,7 +5386,7 @@
         <v>184</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>200</v>
@@ -5377,7 +5422,7 @@
         <v>187</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>188</v>
@@ -5395,7 +5440,7 @@
         <v>189</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>190</v>
@@ -5431,7 +5476,7 @@
         <v>192</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>193</v>
@@ -5485,7 +5530,7 @@
         <v>196</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>197</v>
@@ -5765,7 +5810,7 @@
         <v>217</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>218</v>
@@ -6047,7 +6092,7 @@
         <v>289</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>290</v>
@@ -6064,8 +6109,8 @@
       <c r="B46" s="42" t="s">
         <v>292</v>
       </c>
-      <c r="C46" s="41" t="s">
-        <v>3</v>
+      <c r="C46" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="D46" s="42" t="s">
         <v>293</v>
@@ -6083,7 +6128,7 @@
         <v>295</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>193</v>
@@ -6100,8 +6145,8 @@
       <c r="B48" s="33" t="s">
         <v>296</v>
       </c>
-      <c r="C48" s="30" t="s">
-        <v>3</v>
+      <c r="C48" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="D48" s="31" t="s">
         <v>297</v>
@@ -6119,7 +6164,7 @@
         <v>298</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>211</v>
@@ -6137,7 +6182,7 @@
         <v>299</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>214</v>
@@ -6155,7 +6200,7 @@
         <v>300</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D51" t="s">
         <v>279</v>

</xml_diff>

<commit_message>
Added and not active: TID_GLOBAL_EVENT_HALLOWEEN_DISGUISE TID_GLOBAL_EVENT_BATS TID_GLOBAL_EVENT_WITCH
Former-commit-id: bebf165dbb22972b9424183d0eb766a460fe845f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="396">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -1200,6 +1200,21 @@
   </si>
   <si>
     <t>TID_GLOBAL_EVENT_HALLOWEEN_HATS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TID_GLOBAL_EVENT_HALLOWEEN_DISGUISE</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_BATS</t>
+  </si>
+  <si>
+    <t>BatSmall_Flock;BatBig_Flock</t>
+  </si>
+  <si>
+    <t>icon_bat_s</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_WITCH</t>
   </si>
 </sst>
 </file>
@@ -1304,7 +1319,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1386,11 +1401,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1490,6 +1518,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1772,7 +1803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G178"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
+    <sheetView topLeftCell="A111" workbookViewId="0">
       <selection activeCell="G106" activeCellId="2" sqref="C106 E106 G106"/>
     </sheetView>
   </sheetViews>
@@ -5538,10 +5569,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A63" sqref="A61:A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6605,6 +6636,54 @@
         <v>246</v>
       </c>
     </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="9"/>
+      <c r="B61" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="E61" s="9"/>
+      <c r="F61" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="9"/>
+      <c r="B62" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="E62" s="9"/>
+      <c r="F62" s="45" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="9"/>
+      <c r="B63" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E63" s="9"/>
+      <c r="F63" s="45" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tournament fix icon_eat_gold instead of icon_golden Icon_freeze instead of icon_frozen icon_stun instead of icon_stunned eat_gold instead of kill_golden
activated some quest with tids


Former-commit-id: 02da75810ae4b111632448520688e29ff81c1315
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Tournaments.xlsx
+++ b/Docs/Content/HungryDragonContent_Tournaments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="22125" windowHeight="8475" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="22125" windowHeight="8475"/>
   </bookViews>
   <sheets>
     <sheet name="tournaments" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="395">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -467,9 +467,6 @@
     <t>TID_EVENT_TOURNAMENT_KILL_STUNNED_TIME_ATTACK_ALL</t>
   </si>
   <si>
-    <t>icon_stunned</t>
-  </si>
-  <si>
     <t>TID_EVENT_TOURNAMENT_KILL_FROZEN_NORMAL_ALL</t>
   </si>
   <si>
@@ -479,9 +476,6 @@
     <t>TID_EVENT_TOURNAMENT_KILL_FROZEN_TIME_ATTACK_ALL</t>
   </si>
   <si>
-    <t>icon_frozen</t>
-  </si>
-  <si>
     <t>TID_EVENT_TOURNAMENT_NORMAL_HUNGRY_BIRTHDAY_MODE</t>
   </si>
   <si>
@@ -569,12 +563,6 @@
     <t>TID_EVENT_TOURNAMENT_KILL_GOLDEN_TIME_ATTACK_ALL</t>
   </si>
   <si>
-    <t>kill_golden</t>
-  </si>
-  <si>
-    <t>icon_golden</t>
-  </si>
-  <si>
     <t>TID_GLOBAL_EVENT_PUMPKINS</t>
   </si>
   <si>
@@ -1215,6 +1203,15 @@
   </si>
   <si>
     <t>TID_GLOBAL_EVENT_WITCH</t>
+  </si>
+  <si>
+    <t>icon_freeze</t>
+  </si>
+  <si>
+    <t>icon_stun</t>
+  </si>
+  <si>
+    <t>eat_gold</t>
   </si>
 </sst>
 </file>
@@ -1803,8 +1800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G178"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="G106" activeCellId="2" sqref="C106 E106 G106"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97:C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2014,7 +2011,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>66</v>
@@ -2037,7 +2034,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>66</v>
@@ -2060,7 +2057,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>66</v>
@@ -2077,7 +2074,7 @@
         <v>69</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D14" s="9">
         <v>0</v>
@@ -2240,7 +2237,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="11" t="s">
@@ -2261,7 +2258,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="11" t="s">
@@ -2282,7 +2279,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="11" t="s">
@@ -2672,7 +2669,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="11" t="s">
@@ -2693,7 +2690,7 @@
         <v>2</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="11" t="s">
@@ -2714,7 +2711,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="11" t="s">
@@ -2735,7 +2732,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F44" s="9" t="s">
         <v>115</v>
@@ -2758,7 +2755,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>115</v>
@@ -2781,7 +2778,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F46" s="9" t="s">
         <v>115</v>
@@ -2924,7 +2921,7 @@
         <v>123</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D53" s="9">
         <v>0</v>
@@ -2943,7 +2940,7 @@
         <v>124</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D54" s="9">
         <v>2</v>
@@ -2962,7 +2959,7 @@
         <v>125</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D55" s="9">
         <v>1</v>
@@ -2981,7 +2978,7 @@
         <v>126</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D56" s="9">
         <v>0</v>
@@ -3000,7 +2997,7 @@
         <v>127</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D57" s="9">
         <v>2</v>
@@ -3019,7 +3016,7 @@
         <v>128</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D58" s="9">
         <v>1</v>
@@ -3044,7 +3041,7 @@
         <v>0</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="11" t="s">
@@ -3065,7 +3062,7 @@
         <v>2</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F60" s="9"/>
       <c r="G60" s="11" t="s">
@@ -3086,7 +3083,7 @@
         <v>1</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F61" s="9"/>
       <c r="G61" s="11" t="s">
@@ -3170,7 +3167,7 @@
         <v>0</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F65" s="9"/>
       <c r="G65" s="11" t="s">
@@ -3191,7 +3188,7 @@
         <v>2</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F66" s="9"/>
       <c r="G66" s="11" t="s">
@@ -3212,7 +3209,7 @@
         <v>1</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F67" s="9"/>
       <c r="G67" s="11" t="s">
@@ -3302,11 +3299,11 @@
         <v>0</v>
       </c>
       <c r="E71" s="20" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F71" s="9"/>
       <c r="G71" s="9" t="s">
-        <v>146</v>
+        <v>393</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3323,11 +3320,11 @@
         <v>2</v>
       </c>
       <c r="E72" s="20" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F72" s="9"/>
       <c r="G72" s="9" t="s">
-        <v>146</v>
+        <v>393</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3344,11 +3341,11 @@
         <v>1</v>
       </c>
       <c r="E73" s="20" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F73" s="9"/>
       <c r="G73" s="9" t="s">
-        <v>146</v>
+        <v>393</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3356,7 +3353,7 @@
         <v>0</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>32</v>
@@ -3365,11 +3362,11 @@
         <v>0</v>
       </c>
       <c r="E74" s="20" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F74" s="9"/>
       <c r="G74" s="9" t="s">
-        <v>150</v>
+        <v>392</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3377,7 +3374,7 @@
         <v>0</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C75" s="9" t="s">
         <v>32</v>
@@ -3386,11 +3383,11 @@
         <v>2</v>
       </c>
       <c r="E75" s="20" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F75" s="9"/>
       <c r="G75" s="9" t="s">
-        <v>150</v>
+        <v>392</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -3398,7 +3395,7 @@
         <v>0</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>32</v>
@@ -3407,11 +3404,11 @@
         <v>1</v>
       </c>
       <c r="E76" s="20" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F76" s="9"/>
       <c r="G76" s="9" t="s">
-        <v>150</v>
+        <v>392</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -3419,7 +3416,7 @@
         <v>0</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C77" s="12" t="s">
         <v>46</v>
@@ -3457,7 +3454,7 @@
         <v>0</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>46</v>
@@ -3476,7 +3473,7 @@
         <v>0</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C80" s="12" t="s">
         <v>48</v>
@@ -3514,7 +3511,7 @@
         <v>0</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C82" s="9" t="s">
         <v>7</v>
@@ -3523,13 +3520,13 @@
         <v>0</v>
       </c>
       <c r="E82" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F82" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F82" s="9" t="s">
-        <v>160</v>
-      </c>
       <c r="G82" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3537,7 +3534,7 @@
         <v>0</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>7</v>
@@ -3546,13 +3543,13 @@
         <v>2</v>
       </c>
       <c r="E83" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F83" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F83" s="9" t="s">
-        <v>160</v>
-      </c>
       <c r="G83" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3560,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C84" s="9" t="s">
         <v>7</v>
@@ -3569,13 +3566,13 @@
         <v>1</v>
       </c>
       <c r="E84" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F84" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F84" s="9" t="s">
-        <v>160</v>
-      </c>
       <c r="G84" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3583,7 +3580,7 @@
         <v>0</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C85" s="9" t="s">
         <v>7</v>
@@ -3604,7 +3601,7 @@
         <v>0</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C86" s="9" t="s">
         <v>7</v>
@@ -3625,7 +3622,7 @@
         <v>0</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C87" s="9" t="s">
         <v>7</v>
@@ -3646,7 +3643,7 @@
         <v>0</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C88" s="9" t="s">
         <v>7</v>
@@ -3655,10 +3652,10 @@
         <v>0</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G88" s="11" t="s">
         <v>39</v>
@@ -3669,7 +3666,7 @@
         <v>0</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C89" s="9" t="s">
         <v>7</v>
@@ -3678,10 +3675,10 @@
         <v>2</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F89" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G89" s="11" t="s">
         <v>39</v>
@@ -3692,7 +3689,7 @@
         <v>0</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C90" s="9" t="s">
         <v>7</v>
@@ -3701,10 +3698,10 @@
         <v>1</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G90" s="11" t="s">
         <v>39</v>
@@ -3715,7 +3712,7 @@
         <v>0</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C91" s="9" t="s">
         <v>7</v>
@@ -3724,7 +3721,7 @@
         <v>0</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F91" s="9"/>
       <c r="G91" s="11" t="s">
@@ -3736,7 +3733,7 @@
         <v>0</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C92" s="9" t="s">
         <v>7</v>
@@ -3745,7 +3742,7 @@
         <v>2</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F92" s="9"/>
       <c r="G92" s="11" t="s">
@@ -3757,7 +3754,7 @@
         <v>0</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C93" s="9" t="s">
         <v>7</v>
@@ -3766,7 +3763,7 @@
         <v>1</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F93" s="9"/>
       <c r="G93" s="11" t="s">
@@ -3778,7 +3775,7 @@
         <v>0</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C94" s="9" t="s">
         <v>33</v>
@@ -3787,7 +3784,7 @@
         <v>0</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F94" s="9"/>
       <c r="G94" s="11" t="s">
@@ -3799,7 +3796,7 @@
         <v>0</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C95" s="9" t="s">
         <v>33</v>
@@ -3808,7 +3805,7 @@
         <v>2</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F95" s="9"/>
       <c r="G95" s="11" t="s">
@@ -3820,7 +3817,7 @@
         <v>0</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C96" s="9" t="s">
         <v>33</v>
@@ -3829,7 +3826,7 @@
         <v>1</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F96" s="9"/>
       <c r="G96" s="11" t="s">
@@ -3841,20 +3838,20 @@
         <v>0</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>180</v>
+        <v>394</v>
       </c>
       <c r="D97" s="9">
         <v>0</v>
       </c>
       <c r="E97" s="20" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F97" s="9"/>
       <c r="G97" s="9" t="s">
-        <v>181</v>
+        <v>235</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3862,20 +3859,20 @@
         <v>0</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>180</v>
+        <v>394</v>
       </c>
       <c r="D98" s="9">
         <v>2</v>
       </c>
       <c r="E98" s="20" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F98" s="9"/>
       <c r="G98" s="9" t="s">
-        <v>181</v>
+        <v>235</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3883,20 +3880,20 @@
         <v>0</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>180</v>
+        <v>394</v>
       </c>
       <c r="D99" s="9">
         <v>1</v>
       </c>
       <c r="E99" s="20" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F99" s="9"/>
       <c r="G99" s="9" t="s">
-        <v>181</v>
+        <v>235</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3904,7 +3901,7 @@
         <v>0</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C100" s="9" t="s">
         <v>7</v>
@@ -3913,11 +3910,11 @@
         <v>0</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="F100" s="9"/>
       <c r="G100" s="12" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3925,7 +3922,7 @@
         <v>0</v>
       </c>
       <c r="B101" s="13" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C101" s="9" t="s">
         <v>7</v>
@@ -3934,11 +3931,11 @@
         <v>2</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="F101" s="9"/>
       <c r="G101" s="12" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3946,7 +3943,7 @@
         <v>0</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C102" s="9" t="s">
         <v>7</v>
@@ -3955,11 +3952,11 @@
         <v>1</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="F102" s="9"/>
       <c r="G102" s="12" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3967,7 +3964,7 @@
         <v>0</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C103" s="9" t="s">
         <v>7</v>
@@ -3976,11 +3973,11 @@
         <v>0</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F103" s="9"/>
       <c r="G103" s="12" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3988,7 +3985,7 @@
         <v>0</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C104" s="9" t="s">
         <v>7</v>
@@ -3997,11 +3994,11 @@
         <v>2</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F104" s="9"/>
       <c r="G104" s="12" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -4009,7 +4006,7 @@
         <v>0</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C105" s="9" t="s">
         <v>7</v>
@@ -4018,11 +4015,11 @@
         <v>1</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F105" s="9"/>
       <c r="G105" s="12" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -4030,7 +4027,7 @@
         <v>0</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C106" s="9" t="s">
         <v>33</v>
@@ -4039,13 +4036,13 @@
         <v>0</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F106" s="9" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G106" s="12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -4053,7 +4050,7 @@
         <v>0</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C107" s="9" t="s">
         <v>33</v>
@@ -4062,13 +4059,13 @@
         <v>2</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G107" s="12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -4076,7 +4073,7 @@
         <v>0</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C108" s="9" t="s">
         <v>33</v>
@@ -4085,13 +4082,13 @@
         <v>1</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G108" s="12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -4099,7 +4096,7 @@
         <v>0</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C109" s="9" t="s">
         <v>33</v>
@@ -4108,11 +4105,11 @@
         <v>0</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F109" s="9"/>
       <c r="G109" s="21" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -4120,7 +4117,7 @@
         <v>0</v>
       </c>
       <c r="B110" s="23" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C110" s="9" t="s">
         <v>33</v>
@@ -4129,11 +4126,11 @@
         <v>2</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F110" s="9"/>
       <c r="G110" s="21" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -4141,7 +4138,7 @@
         <v>0</v>
       </c>
       <c r="B111" s="25" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C111" s="9" t="s">
         <v>7</v>
@@ -4150,11 +4147,11 @@
         <v>2</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F111" s="9"/>
       <c r="G111" s="9" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -4162,7 +4159,7 @@
         <v>0</v>
       </c>
       <c r="B112" s="25" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C112" s="9" t="s">
         <v>7</v>
@@ -4171,11 +4168,11 @@
         <v>0</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F112" s="9"/>
       <c r="G112" s="9" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -4183,7 +4180,7 @@
         <v>0</v>
       </c>
       <c r="B113" s="26" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C113" s="9" t="s">
         <v>7</v>
@@ -4192,11 +4189,11 @@
         <v>1</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F113" s="9"/>
       <c r="G113" s="9" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -4204,7 +4201,7 @@
         <v>0</v>
       </c>
       <c r="B114" s="25" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C114" s="9" t="s">
         <v>7</v>
@@ -4213,11 +4210,11 @@
         <v>2</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F114" s="9"/>
       <c r="G114" s="12" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -4225,7 +4222,7 @@
         <v>0</v>
       </c>
       <c r="B115" s="25" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C115" s="9" t="s">
         <v>7</v>
@@ -4234,11 +4231,11 @@
         <v>0</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F115" s="9"/>
       <c r="G115" s="12" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -4246,7 +4243,7 @@
         <v>0</v>
       </c>
       <c r="B116" s="26" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C116" s="9" t="s">
         <v>7</v>
@@ -4255,11 +4252,11 @@
         <v>1</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F116" s="9"/>
       <c r="G116" s="12" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -4267,7 +4264,7 @@
         <v>0</v>
       </c>
       <c r="B117" s="27" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C117" s="9" t="s">
         <v>7</v>
@@ -4276,11 +4273,11 @@
         <v>2</v>
       </c>
       <c r="E117" s="28" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F117" s="9"/>
       <c r="G117" s="12" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -4288,7 +4285,7 @@
         <v>0</v>
       </c>
       <c r="B118" s="27" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C118" s="9" t="s">
         <v>7</v>
@@ -4297,11 +4294,11 @@
         <v>0</v>
       </c>
       <c r="E118" s="28" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F118" s="9"/>
       <c r="G118" s="12" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="119" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -4309,7 +4306,7 @@
         <v>0</v>
       </c>
       <c r="B119" s="35" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C119" s="30" t="s">
         <v>7</v>
@@ -4318,11 +4315,11 @@
         <v>0</v>
       </c>
       <c r="E119" s="31" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F119" s="30"/>
       <c r="G119" s="30" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -4330,7 +4327,7 @@
         <v>0</v>
       </c>
       <c r="B120" s="24" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C120" s="9" t="s">
         <v>7</v>
@@ -4339,11 +4336,11 @@
         <v>2</v>
       </c>
       <c r="E120" s="7" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F120" s="9"/>
       <c r="G120" s="9" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -4351,7 +4348,7 @@
         <v>0</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C121" s="9" t="s">
         <v>7</v>
@@ -4360,11 +4357,11 @@
         <v>1</v>
       </c>
       <c r="E121" s="7" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F121" s="9"/>
       <c r="G121" s="9" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -4372,7 +4369,7 @@
         <v>0</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C122" s="9" t="s">
         <v>7</v>
@@ -4381,11 +4378,11 @@
         <v>0</v>
       </c>
       <c r="E122" s="7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F122" s="9"/>
       <c r="G122" s="9" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -4393,7 +4390,7 @@
         <v>0</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C123" s="9" t="s">
         <v>7</v>
@@ -4402,11 +4399,11 @@
         <v>2</v>
       </c>
       <c r="E123" s="7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F123" s="9"/>
       <c r="G123" s="9" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -4414,7 +4411,7 @@
         <v>0</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C124" s="9" t="s">
         <v>7</v>
@@ -4423,11 +4420,11 @@
         <v>1</v>
       </c>
       <c r="E124" s="7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F124" s="9"/>
       <c r="G124" s="9" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -4435,7 +4432,7 @@
         <v>0</v>
       </c>
       <c r="B125" s="13" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C125" s="9" t="s">
         <v>7</v>
@@ -4444,11 +4441,11 @@
         <v>0</v>
       </c>
       <c r="E125" s="7" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F125" s="9"/>
       <c r="G125" s="9" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -4456,7 +4453,7 @@
         <v>0</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C126" s="9" t="s">
         <v>7</v>
@@ -4465,11 +4462,11 @@
         <v>2</v>
       </c>
       <c r="E126" s="7" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F126" s="9"/>
       <c r="G126" s="9" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -4477,7 +4474,7 @@
         <v>0</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C127" s="9" t="s">
         <v>7</v>
@@ -4486,11 +4483,11 @@
         <v>1</v>
       </c>
       <c r="E127" s="7" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F127" s="9"/>
       <c r="G127" s="9" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4498,7 +4495,7 @@
         <v>0</v>
       </c>
       <c r="B128" s="13" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C128" s="9" t="s">
         <v>7</v>
@@ -4507,11 +4504,11 @@
         <v>0</v>
       </c>
       <c r="E128" s="7" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F128" s="9"/>
       <c r="G128" s="9" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -4519,7 +4516,7 @@
         <v>0</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C129" s="9" t="s">
         <v>7</v>
@@ -4528,11 +4525,11 @@
         <v>2</v>
       </c>
       <c r="E129" s="7" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F129" s="9"/>
       <c r="G129" s="9" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -4540,7 +4537,7 @@
         <v>0</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C130" s="9" t="s">
         <v>7</v>
@@ -4549,11 +4546,11 @@
         <v>0</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F130" s="9"/>
       <c r="G130" s="9" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -4561,7 +4558,7 @@
         <v>0</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C131" s="9" t="s">
         <v>7</v>
@@ -4570,11 +4567,11 @@
         <v>2</v>
       </c>
       <c r="E131" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F131" s="9"/>
       <c r="G131" s="9" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -4582,7 +4579,7 @@
         <v>0</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C132" s="9" t="s">
         <v>7</v>
@@ -4591,11 +4588,11 @@
         <v>1</v>
       </c>
       <c r="E132" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F132" s="9"/>
       <c r="G132" s="9" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="133" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4603,7 +4600,7 @@
         <v>0</v>
       </c>
       <c r="B133" s="37" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C133" s="36" t="s">
         <v>7</v>
@@ -4612,11 +4609,11 @@
         <v>1</v>
       </c>
       <c r="E133" s="37" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F133" s="36"/>
       <c r="G133" s="36" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="134" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4624,7 +4621,7 @@
         <v>0</v>
       </c>
       <c r="B134" s="37" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C134" s="36" t="s">
         <v>7</v>
@@ -4633,11 +4630,11 @@
         <v>2</v>
       </c>
       <c r="E134" s="37" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F134" s="36"/>
       <c r="G134" s="36" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="135" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4645,7 +4642,7 @@
         <v>0</v>
       </c>
       <c r="B135" s="37" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C135" s="36" t="s">
         <v>7</v>
@@ -4654,11 +4651,11 @@
         <v>1</v>
       </c>
       <c r="E135" s="37" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F135" s="36"/>
       <c r="G135" s="36" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -4666,7 +4663,7 @@
         <v>0</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C136" s="9" t="s">
         <v>7</v>
@@ -4675,11 +4672,11 @@
         <v>0</v>
       </c>
       <c r="E136" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F136" s="9"/>
       <c r="G136" s="9" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -4687,7 +4684,7 @@
         <v>0</v>
       </c>
       <c r="B137" s="13" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C137" s="9" t="s">
         <v>7</v>
@@ -4696,11 +4693,11 @@
         <v>2</v>
       </c>
       <c r="E137" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F137" s="9"/>
       <c r="G137" s="9" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -4708,7 +4705,7 @@
         <v>0</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C138" s="9" t="s">
         <v>7</v>
@@ -4717,11 +4714,11 @@
         <v>1</v>
       </c>
       <c r="E138" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F138" s="9"/>
       <c r="G138" s="9" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="139" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4729,7 +4726,7 @@
         <v>0</v>
       </c>
       <c r="B139" s="37" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C139" s="9" t="s">
         <v>7</v>
@@ -4738,7 +4735,7 @@
         <v>2</v>
       </c>
       <c r="E139" s="37" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F139" s="36"/>
       <c r="G139" s="36" t="s">
@@ -4750,7 +4747,7 @@
         <v>0</v>
       </c>
       <c r="B140" s="37" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C140" s="9" t="s">
         <v>7</v>
@@ -4759,7 +4756,7 @@
         <v>0</v>
       </c>
       <c r="E140" s="37" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F140" s="36"/>
       <c r="G140" s="36" t="s">
@@ -4771,7 +4768,7 @@
         <v>0</v>
       </c>
       <c r="B141" s="37" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C141" s="36" t="s">
         <v>46</v>
@@ -4780,7 +4777,7 @@
         <v>2</v>
       </c>
       <c r="E141" s="37" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F141" s="36"/>
       <c r="G141" s="36" t="s">
@@ -4792,7 +4789,7 @@
         <v>0</v>
       </c>
       <c r="B142" s="37" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C142" s="36" t="s">
         <v>48</v>
@@ -4801,7 +4798,7 @@
         <v>2</v>
       </c>
       <c r="E142" s="37" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F142" s="36"/>
       <c r="G142" s="36" t="s">
@@ -4813,7 +4810,7 @@
         <v>0</v>
       </c>
       <c r="B143" s="37" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C143" s="36" t="s">
         <v>46</v>
@@ -4822,7 +4819,7 @@
         <v>0</v>
       </c>
       <c r="E143" s="37" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F143" s="36"/>
       <c r="G143" s="36" t="s">
@@ -4834,7 +4831,7 @@
         <v>0</v>
       </c>
       <c r="B144" s="37" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C144" s="36" t="s">
         <v>46</v>
@@ -4843,7 +4840,7 @@
         <v>1</v>
       </c>
       <c r="E144" s="37" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F144" s="36"/>
       <c r="G144" s="36" t="s">
@@ -4855,7 +4852,7 @@
         <v>0</v>
       </c>
       <c r="B145" s="37" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C145" s="36" t="s">
         <v>48</v>
@@ -4864,7 +4861,7 @@
         <v>0</v>
       </c>
       <c r="E145" s="37" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F145" s="36"/>
       <c r="G145" s="36" t="s">
@@ -4876,7 +4873,7 @@
         <v>0</v>
       </c>
       <c r="B146" s="37" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C146" s="36" t="s">
         <v>7</v>
@@ -4885,11 +4882,11 @@
         <v>2</v>
       </c>
       <c r="E146" s="37" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F146" s="36"/>
       <c r="G146" s="36" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="147" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4897,7 +4894,7 @@
         <v>0</v>
       </c>
       <c r="B147" s="37" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C147" s="36" t="s">
         <v>7</v>
@@ -4906,11 +4903,11 @@
         <v>0</v>
       </c>
       <c r="E147" s="37" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F147" s="36"/>
       <c r="G147" s="36" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="148" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4918,7 +4915,7 @@
         <v>0</v>
       </c>
       <c r="B148" s="37" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C148" s="36" t="s">
         <v>46</v>
@@ -4927,11 +4924,11 @@
         <v>2</v>
       </c>
       <c r="E148" s="37" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F148" s="36"/>
       <c r="G148" s="36" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="149" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4939,7 +4936,7 @@
         <v>0</v>
       </c>
       <c r="B149" s="37" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C149" s="36" t="s">
         <v>48</v>
@@ -4948,11 +4945,11 @@
         <v>2</v>
       </c>
       <c r="E149" s="37" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F149" s="36"/>
       <c r="G149" s="36" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="150" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4960,7 +4957,7 @@
         <v>0</v>
       </c>
       <c r="B150" s="37" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C150" s="36" t="s">
         <v>46</v>
@@ -4969,11 +4966,11 @@
         <v>0</v>
       </c>
       <c r="E150" s="37" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F150" s="36"/>
       <c r="G150" s="36" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="151" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4981,7 +4978,7 @@
         <v>0</v>
       </c>
       <c r="B151" s="37" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C151" s="36" t="s">
         <v>46</v>
@@ -4990,11 +4987,11 @@
         <v>1</v>
       </c>
       <c r="E151" s="37" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F151" s="36"/>
       <c r="G151" s="36" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="152" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -5002,7 +4999,7 @@
         <v>0</v>
       </c>
       <c r="B152" s="37" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C152" s="36" t="s">
         <v>48</v>
@@ -5011,11 +5008,11 @@
         <v>0</v>
       </c>
       <c r="E152" s="37" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F152" s="36"/>
       <c r="G152" s="36" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="153" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -5023,7 +5020,7 @@
         <v>0</v>
       </c>
       <c r="B153" s="39" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C153" s="36" t="s">
         <v>7</v>
@@ -5032,11 +5029,11 @@
         <v>0</v>
       </c>
       <c r="E153" s="37" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F153" s="36"/>
       <c r="G153" s="36" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="154" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -5044,7 +5041,7 @@
         <v>0</v>
       </c>
       <c r="B154" s="40" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C154" s="36" t="s">
         <v>7</v>
@@ -5053,11 +5050,11 @@
         <v>2</v>
       </c>
       <c r="E154" s="37" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F154" s="36"/>
       <c r="G154" s="36" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="155" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -5065,7 +5062,7 @@
         <v>0</v>
       </c>
       <c r="B155" s="37" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C155" s="36" t="s">
         <v>7</v>
@@ -5074,11 +5071,11 @@
         <v>1</v>
       </c>
       <c r="E155" s="37" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F155" s="36"/>
       <c r="G155" s="36" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -5086,7 +5083,7 @@
         <v>0</v>
       </c>
       <c r="B156" s="13" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C156" s="9" t="s">
         <v>7</v>
@@ -5095,11 +5092,11 @@
         <v>0</v>
       </c>
       <c r="E156" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F156" s="9"/>
       <c r="G156" s="12" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -5107,7 +5104,7 @@
         <v>0</v>
       </c>
       <c r="B157" s="13" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C157" s="9" t="s">
         <v>7</v>
@@ -5116,11 +5113,11 @@
         <v>2</v>
       </c>
       <c r="E157" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F157" s="9"/>
       <c r="G157" s="12" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -5128,7 +5125,7 @@
         <v>0</v>
       </c>
       <c r="B158" s="13" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C158" s="9" t="s">
         <v>7</v>
@@ -5137,11 +5134,11 @@
         <v>1</v>
       </c>
       <c r="E158" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F158" s="9"/>
       <c r="G158" s="12" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -5149,7 +5146,7 @@
         <v>0</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C159" s="9" t="s">
         <v>7</v>
@@ -5158,11 +5155,11 @@
         <v>0</v>
       </c>
       <c r="E159" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F159" s="9"/>
       <c r="G159" s="12" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -5170,7 +5167,7 @@
         <v>0</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C160" s="9" t="s">
         <v>7</v>
@@ -5179,11 +5176,11 @@
         <v>2</v>
       </c>
       <c r="E160" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F160" s="9"/>
       <c r="G160" s="12" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -5191,7 +5188,7 @@
         <v>0</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C161" s="9" t="s">
         <v>7</v>
@@ -5200,11 +5197,11 @@
         <v>1</v>
       </c>
       <c r="E161" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F161" s="9"/>
       <c r="G161" s="12" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -5212,7 +5209,7 @@
         <v>0</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C162" s="9" t="s">
         <v>33</v>
@@ -5221,10 +5218,10 @@
         <v>2</v>
       </c>
       <c r="E162" s="7" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G162" s="11" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
@@ -5232,7 +5229,7 @@
         <v>0</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C163" s="9" t="s">
         <v>33</v>
@@ -5241,11 +5238,11 @@
         <v>0</v>
       </c>
       <c r="E163" s="7" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="F163" s="9"/>
       <c r="G163" s="11" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -5253,7 +5250,7 @@
         <v>0</v>
       </c>
       <c r="B164" s="13" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C164" s="9" t="s">
         <v>33</v>
@@ -5262,11 +5259,11 @@
         <v>1</v>
       </c>
       <c r="E164" s="7" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="F164" s="9"/>
       <c r="G164" s="11" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
@@ -5274,7 +5271,7 @@
         <v>0</v>
       </c>
       <c r="B165" s="13" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C165" s="9" t="s">
         <v>7</v>
@@ -5283,10 +5280,10 @@
         <v>2</v>
       </c>
       <c r="E165" s="7" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="G165" s="12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -5294,7 +5291,7 @@
         <v>0</v>
       </c>
       <c r="B166" s="13" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C166" s="9" t="s">
         <v>7</v>
@@ -5303,11 +5300,11 @@
         <v>0</v>
       </c>
       <c r="E166" s="7" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="F166" s="9"/>
       <c r="G166" s="12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -5315,7 +5312,7 @@
         <v>0</v>
       </c>
       <c r="B167" s="13" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C167" s="9" t="s">
         <v>7</v>
@@ -5324,11 +5321,11 @@
         <v>1</v>
       </c>
       <c r="E167" s="7" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="F167" s="9"/>
       <c r="G167" s="12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="168" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -5336,7 +5333,7 @@
         <v>0</v>
       </c>
       <c r="B168" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C168" s="9" t="s">
         <v>7</v>
@@ -5345,7 +5342,7 @@
         <v>2</v>
       </c>
       <c r="E168" s="37" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F168" s="36"/>
       <c r="G168" s="36" t="s">
@@ -5357,7 +5354,7 @@
         <v>0</v>
       </c>
       <c r="B169" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C169" s="9" t="s">
         <v>7</v>
@@ -5366,7 +5363,7 @@
         <v>0</v>
       </c>
       <c r="E169" s="37" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F169" s="36"/>
       <c r="G169" s="36" t="s">
@@ -5378,7 +5375,7 @@
         <v>0</v>
       </c>
       <c r="B170" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C170" s="9" t="s">
         <v>7</v>
@@ -5387,7 +5384,7 @@
         <v>0</v>
       </c>
       <c r="E170" s="7" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="F170" s="9"/>
       <c r="G170" s="11" t="s">
@@ -5399,7 +5396,7 @@
         <v>0</v>
       </c>
       <c r="B171" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C171" s="9" t="s">
         <v>7</v>
@@ -5408,7 +5405,7 @@
         <v>2</v>
       </c>
       <c r="E171" s="7" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="F171" s="9"/>
       <c r="G171" s="11" t="s">
@@ -5420,7 +5417,7 @@
         <v>0</v>
       </c>
       <c r="B172" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C172" s="9" t="s">
         <v>7</v>
@@ -5429,7 +5426,7 @@
         <v>1</v>
       </c>
       <c r="E172" s="7" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="F172" s="9"/>
       <c r="G172" s="11" t="s">
@@ -5441,7 +5438,7 @@
         <v>0</v>
       </c>
       <c r="B173" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C173" s="9" t="s">
         <v>33</v>
@@ -5450,10 +5447,10 @@
         <v>2</v>
       </c>
       <c r="E173" s="7" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="G173" s="12" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
@@ -5461,7 +5458,7 @@
         <v>0</v>
       </c>
       <c r="B174" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C174" s="9" t="s">
         <v>33</v>
@@ -5470,11 +5467,11 @@
         <v>0</v>
       </c>
       <c r="E174" s="7" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F174" s="9"/>
       <c r="G174" s="12" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -5482,7 +5479,7 @@
         <v>0</v>
       </c>
       <c r="B175" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C175" s="9" t="s">
         <v>33</v>
@@ -5491,11 +5488,11 @@
         <v>1</v>
       </c>
       <c r="E175" s="7" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F175" s="9"/>
       <c r="G175" s="12" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -5503,7 +5500,7 @@
         <v>0</v>
       </c>
       <c r="B176" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C176" s="9" t="s">
         <v>33</v>
@@ -5512,11 +5509,11 @@
         <v>2</v>
       </c>
       <c r="E176" s="7" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="F176" s="9"/>
       <c r="G176" s="12" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
@@ -5524,7 +5521,7 @@
         <v>0</v>
       </c>
       <c r="B177" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="C177" s="9" t="s">
         <v>33</v>
@@ -5533,11 +5530,11 @@
         <v>0</v>
       </c>
       <c r="E177" s="7" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="F177" s="9"/>
       <c r="G177" s="12" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
@@ -5545,7 +5542,7 @@
         <v>0</v>
       </c>
       <c r="B178" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C178" s="9" t="s">
         <v>33</v>
@@ -5554,11 +5551,11 @@
         <v>1</v>
       </c>
       <c r="E178" s="7" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="F178" s="9"/>
       <c r="G178" s="12" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -5571,8 +5568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A63" sqref="A61:A63"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5588,7 +5585,7 @@
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -5604,7 +5601,7 @@
     </row>
     <row r="4" spans="1:6" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -5627,19 +5624,19 @@
         <v>0</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -5647,17 +5644,17 @@
         <v>0</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="12" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -5665,17 +5662,17 @@
         <v>0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="12" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -5683,17 +5680,17 @@
         <v>0</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="12" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -5701,17 +5698,17 @@
         <v>0</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="12" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -5719,13 +5716,13 @@
         <v>0</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="12" t="s">
@@ -5737,17 +5734,17 @@
         <v>0</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="12" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -5755,7 +5752,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>29</v>
@@ -5775,7 +5772,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>2</v>
@@ -5791,17 +5788,17 @@
         <v>0</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="12" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -5809,7 +5806,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>4</v>
@@ -5825,7 +5822,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>3</v>
@@ -5843,7 +5840,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>46</v>
@@ -5859,13 +5856,13 @@
         <v>0</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>66</v>
@@ -5879,7 +5876,7 @@
         <v>0</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>5</v>
@@ -5895,7 +5892,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>2</v>
@@ -5911,17 +5908,17 @@
         <v>0</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="12" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -5929,13 +5926,13 @@
         <v>0</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="12" t="s">
@@ -5947,7 +5944,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>6</v>
@@ -5963,13 +5960,13 @@
         <v>0</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="12" t="s">
@@ -5981,17 +5978,17 @@
         <v>0</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="12" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -5999,13 +5996,13 @@
         <v>0</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="12" t="s">
@@ -6017,13 +6014,13 @@
         <v>0</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="12" t="s">
@@ -6035,7 +6032,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>7</v>
@@ -6053,7 +6050,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>7</v>
@@ -6071,17 +6068,17 @@
         <v>0</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="12" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -6089,7 +6086,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>7</v>
@@ -6109,7 +6106,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>7</v>
@@ -6129,7 +6126,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>7</v>
@@ -6149,7 +6146,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>7</v>
@@ -6169,7 +6166,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>7</v>
@@ -6181,7 +6178,7 @@
         <v>107</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -6189,7 +6186,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>7</v>
@@ -6207,19 +6204,19 @@
         <v>0</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D37" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E37" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E37" s="9" t="s">
-        <v>160</v>
-      </c>
       <c r="F37" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -6227,13 +6224,13 @@
         <v>0</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>115</v>
@@ -6247,7 +6244,7 @@
         <v>0</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>7</v>
@@ -6255,7 +6252,7 @@
       <c r="D39" s="16"/>
       <c r="E39" s="14"/>
       <c r="F39" s="17" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -6263,17 +6260,17 @@
         <v>0</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E40" s="18"/>
       <c r="F40" s="12" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -6281,17 +6278,17 @@
         <v>0</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="12" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -6299,17 +6296,17 @@
         <v>0</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="9" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -6317,17 +6314,17 @@
         <v>0</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="21" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -6335,17 +6332,17 @@
         <v>0</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="12" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -6353,17 +6350,17 @@
         <v>0</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="12" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -6371,17 +6368,17 @@
         <v>0</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D46" s="42" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E46" s="41"/>
       <c r="F46" s="43" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -6389,17 +6386,17 @@
         <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E47" s="9"/>
       <c r="F47" s="12" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -6407,17 +6404,17 @@
         <v>0</v>
       </c>
       <c r="B48" s="33" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E48" s="30"/>
       <c r="F48" s="32" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -6425,17 +6422,17 @@
         <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E49" s="9"/>
       <c r="F49" s="12" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -6443,13 +6440,13 @@
         <v>0</v>
       </c>
       <c r="B50" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E50" s="9"/>
       <c r="F50" s="36" t="s">
@@ -6461,17 +6458,17 @@
         <v>0</v>
       </c>
       <c r="B51" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D51" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E51" s="9"/>
       <c r="F51" s="36" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -6479,17 +6476,17 @@
         <v>0</v>
       </c>
       <c r="B52" s="44" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C52" s="41" t="s">
         <v>7</v>
       </c>
       <c r="D52" s="44" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E52" s="41"/>
       <c r="F52" s="43" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -6497,17 +6494,17 @@
         <v>0</v>
       </c>
       <c r="B53" s="44" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C53" s="41" t="s">
         <v>7</v>
       </c>
       <c r="D53" s="42" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E53" s="41"/>
       <c r="F53" s="43" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -6515,17 +6512,17 @@
         <v>0</v>
       </c>
       <c r="B54" s="44" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C54" s="41" t="s">
         <v>7</v>
       </c>
       <c r="D54" s="42" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E54" s="41"/>
       <c r="F54" s="43" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -6533,17 +6530,17 @@
         <v>0</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E55" s="18"/>
       <c r="F55" s="12" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -6551,17 +6548,17 @@
         <v>0</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="E56" s="18"/>
       <c r="F56" s="12" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -6569,17 +6566,17 @@
         <v>0</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C57" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E57" s="18"/>
       <c r="F57" s="12" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -6587,13 +6584,13 @@
         <v>0</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C58" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="E58" s="9"/>
       <c r="F58" s="12" t="s">
@@ -6605,17 +6602,17 @@
         <v>0</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E59" s="9"/>
       <c r="F59" s="12" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -6623,55 +6620,61 @@
         <v>0</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E60" s="9"/>
       <c r="F60" s="12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="9"/>
+      <c r="A61" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="B61" s="7" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C61" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E61" s="9"/>
       <c r="F61" s="12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="9"/>
+      <c r="A62" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="B62" s="7" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="E62" s="9"/>
       <c r="F62" s="45" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="9"/>
+      <c r="A63" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="B63" s="7" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C63" s="9" t="s">
         <v>7</v>

</xml_diff>